<commit_message>
Remove Duplicate Data, Fill Blank Cells
Blank Cells replaced with 'N/A'
No Duplicate Rows Found
</commit_message>
<xml_diff>
--- a/ARA DATA Wait Lists Feb 2021.xlsx
+++ b/ARA DATA Wait Lists Feb 2021.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JulanRay\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tewaka-my.sharepoint.com/personal/jra0108_arastudent_ac_nz/Documents/2021/Bachelor (Sem2)/BCDE103/Assessment/Assignment 1/Submit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62C6F57-4F11-4DC1-8AB4-9BAEA44BD995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{F62C6F57-4F11-4DC1-8AB4-9BAEA44BD995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BD07DB0-82BE-4B4F-BFC0-62EB4ECC1169}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2250" yWindow="2250" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -2487,7 +2487,7 @@
   <dimension ref="A1:O101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:O1048576"/>
+      <selection activeCell="F12" sqref="A1:N101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Proper Case Formatting Names, Departments etc
</commit_message>
<xml_diff>
--- a/ARA DATA Wait Lists Feb 2021.xlsx
+++ b/ARA DATA Wait Lists Feb 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tewaka-my.sharepoint.com/personal/jra0108_arastudent_ac_nz/Documents/2021/Bachelor (Sem2)/BCDE103/Assessment/Assignment 1/Submit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{F62C6F57-4F11-4DC1-8AB4-9BAEA44BD995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BD07DB0-82BE-4B4F-BFC0-62EB4ECC1169}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{F62C6F57-4F11-4DC1-8AB4-9BAEA44BD995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA0D8261-0C67-4FA4-9593-BA4C3D81E56A}"/>
   <bookViews>
     <workbookView xWindow="2250" yWindow="2250" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -948,9 +948,6 @@
     <t>Evelyn Rae</t>
   </si>
   <si>
-    <t>Greta McLean</t>
-  </si>
-  <si>
     <t>Michael Lewis</t>
   </si>
   <si>
@@ -1044,9 +1041,6 @@
     <t>Scottie Emms</t>
   </si>
   <si>
-    <t>Elicia McCay</t>
-  </si>
-  <si>
     <t>Elvera Peasby</t>
   </si>
   <si>
@@ -1074,21 +1068,9 @@
     <t>Efrem Kippax</t>
   </si>
   <si>
-    <t>Rad MacKaig</t>
-  </si>
-  <si>
-    <t>Smith McGettigan</t>
-  </si>
-  <si>
-    <t>Davida MacCurlye</t>
-  </si>
-  <si>
     <t>Beverie Robez</t>
   </si>
   <si>
-    <t>Shirline Van der Kruys</t>
-  </si>
-  <si>
     <t>Brig Ovendale</t>
   </si>
   <si>
@@ -1266,9 +1248,6 @@
     <t>Flin Gleasane</t>
   </si>
   <si>
-    <t>Chas McGrah</t>
-  </si>
-  <si>
     <t>Sheri Corhard</t>
   </si>
   <si>
@@ -2140,6 +2119,27 @@
   </si>
   <si>
     <t>37969</t>
+  </si>
+  <si>
+    <t>Shirline Van Der Kruys</t>
+  </si>
+  <si>
+    <t>Davida Maccurlye</t>
+  </si>
+  <si>
+    <t>Elicia Mccay</t>
+  </si>
+  <si>
+    <t>Smith Mcgettigan</t>
+  </si>
+  <si>
+    <t>Chas Mcgrah</t>
+  </si>
+  <si>
+    <t>Rad Mackaig</t>
+  </si>
+  <si>
+    <t>Greta Mclean</t>
   </si>
 </sst>
 </file>
@@ -2486,8 +2486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="A1:N101"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2534,22 +2534,22 @@
         <v>6</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>322</v>
-      </c>
       <c r="N1" s="2" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="O1" s="3"/>
     </row>
@@ -2570,10 +2570,10 @@
         <v>129</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>295</v>
@@ -2582,19 +2582,19 @@
         <v>299</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>534</v>
+        <v>527</v>
       </c>
       <c r="K2" t="s">
         <v>205</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>621</v>
+        <v>614</v>
       </c>
       <c r="M2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>684</v>
+        <v>677</v>
       </c>
       <c r="O2" s="3"/>
     </row>
@@ -2615,28 +2615,28 @@
         <v>80</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>349</v>
+        <v>694</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I3" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>534</v>
+        <v>527</v>
       </c>
       <c r="K3" t="s">
         <v>207</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>622</v>
+        <v>615</v>
       </c>
       <c r="M3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>81</v>
@@ -2660,28 +2660,28 @@
         <v>50</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>295</v>
       </c>
       <c r="I4" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
       <c r="K4" t="s">
         <v>206</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>623</v>
+        <v>616</v>
       </c>
       <c r="M4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>51</v>
@@ -2705,28 +2705,28 @@
         <v>177</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>295</v>
       </c>
       <c r="I5" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
       <c r="K5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>624</v>
+        <v>617</v>
       </c>
       <c r="M5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>178</v>
@@ -2750,28 +2750,28 @@
         <v>149</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I6" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
       <c r="K6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>625</v>
+        <v>618</v>
       </c>
       <c r="M6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>150</v>
@@ -2795,28 +2795,28 @@
         <v>169</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>295</v>
       </c>
       <c r="I7" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
       <c r="K7" t="s">
         <v>302</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>626</v>
+        <v>619</v>
       </c>
       <c r="M7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>170</v>
@@ -2840,28 +2840,28 @@
         <v>87</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I8" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="K8" t="s">
         <v>302</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="M8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>88</v>
@@ -2885,28 +2885,28 @@
         <v>58</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>295</v>
       </c>
       <c r="I9" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
       <c r="K9" t="s">
         <v>206</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>627</v>
+        <v>620</v>
       </c>
       <c r="M9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>59</v>
@@ -2930,28 +2930,28 @@
         <v>30</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>295</v>
       </c>
       <c r="I10" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="K10" t="s">
         <v>206</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>628</v>
+        <v>621</v>
       </c>
       <c r="M10" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>31</v>
@@ -2975,28 +2975,28 @@
         <v>95</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>295</v>
       </c>
       <c r="I11" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="K11" t="s">
-        <v>303</v>
+        <v>700</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>546</v>
+        <v>539</v>
       </c>
       <c r="M11" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>96</v>
@@ -3020,31 +3020,31 @@
         <v>72</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I12" t="s">
         <v>300</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="K12" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>629</v>
+        <v>622</v>
       </c>
       <c r="M12" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="O12" s="3"/>
     </row>
@@ -3065,28 +3065,28 @@
         <v>157</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I13" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>544</v>
+        <v>537</v>
       </c>
       <c r="K13" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>630</v>
+        <v>623</v>
       </c>
       <c r="M13" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>158</v>
@@ -3110,28 +3110,28 @@
         <v>183</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I14" t="s">
         <v>299</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>544</v>
+        <v>537</v>
       </c>
       <c r="K14" t="s">
         <v>204</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>631</v>
+        <v>624</v>
       </c>
       <c r="M14" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>184</v>
@@ -3155,10 +3155,10 @@
         <v>134</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>295</v>
@@ -3167,19 +3167,19 @@
         <v>300</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
       <c r="K15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>632</v>
+        <v>625</v>
       </c>
       <c r="M15" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>685</v>
+        <v>678</v>
       </c>
       <c r="O15" s="3"/>
     </row>
@@ -3191,7 +3191,7 @@
         <v>287</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D16" t="s">
         <v>194</v>
@@ -3200,10 +3200,10 @@
         <v>163</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>295</v>
@@ -3212,16 +3212,16 @@
         <v>299</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
       <c r="K16" t="s">
         <v>203</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>633</v>
+        <v>626</v>
       </c>
       <c r="M16" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>164</v>
@@ -3245,31 +3245,31 @@
         <v>36</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I17" t="s">
         <v>300</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>546</v>
+        <v>539</v>
       </c>
       <c r="K17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>634</v>
+        <v>627</v>
       </c>
       <c r="M17" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="O17" s="3"/>
     </row>
@@ -3290,28 +3290,28 @@
         <v>20</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>295</v>
       </c>
       <c r="I18" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
       <c r="K18" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>635</v>
+        <v>628</v>
       </c>
       <c r="M18" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>21</v>
@@ -3335,28 +3335,28 @@
         <v>132</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I19" t="s">
         <v>299</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>548</v>
+        <v>541</v>
       </c>
       <c r="K19" t="s">
         <v>203</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
       <c r="M19" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>133</v>
@@ -3380,28 +3380,28 @@
         <v>48</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I20" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>549</v>
+        <v>542</v>
       </c>
       <c r="K20" t="s">
         <v>301</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>636</v>
+        <v>629</v>
       </c>
       <c r="M20" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>49</v>
@@ -3425,28 +3425,28 @@
         <v>40</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>295</v>
       </c>
       <c r="I21" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>550</v>
+        <v>543</v>
       </c>
       <c r="K21" t="s">
         <v>208</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>565</v>
+        <v>558</v>
       </c>
       <c r="M21" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N21" s="1" t="s">
         <v>41</v>
@@ -3470,28 +3470,28 @@
         <v>191</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I22" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>551</v>
+        <v>544</v>
       </c>
       <c r="K22" t="s">
-        <v>303</v>
+        <v>700</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>637</v>
+        <v>630</v>
       </c>
       <c r="M22" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N22" s="1" t="s">
         <v>192</v>
@@ -3515,31 +3515,31 @@
         <v>84</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="I23" t="s">
         <v>300</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
       <c r="K23" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>638</v>
+        <v>631</v>
       </c>
       <c r="M23" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>686</v>
+        <v>679</v>
       </c>
       <c r="O23" s="3"/>
     </row>
@@ -3560,28 +3560,28 @@
         <v>54</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="H24" s="7" t="s">
         <v>295</v>
       </c>
       <c r="I24" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
       <c r="K24" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>633</v>
+        <v>626</v>
       </c>
       <c r="M24" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N24" s="1" t="s">
         <v>55</v>
@@ -3605,10 +3605,10 @@
         <v>67</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>295</v>
@@ -3617,19 +3617,19 @@
         <v>300</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
       <c r="K25" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>639</v>
+        <v>632</v>
       </c>
       <c r="M25" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N25" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="O25" s="3"/>
     </row>
@@ -3650,28 +3650,28 @@
         <v>73</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I26" t="s">
         <v>299</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>554</v>
+        <v>547</v>
       </c>
       <c r="K26" t="s">
         <v>203</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>567</v>
+        <v>560</v>
       </c>
       <c r="M26" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N26" s="1" t="s">
         <v>74</v>
@@ -3695,31 +3695,31 @@
         <v>25</v>
       </c>
       <c r="F27" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>450</v>
+      </c>
+      <c r="H27" s="7" t="s">
         <v>327</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>457</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>328</v>
       </c>
       <c r="I27" t="s">
         <v>300</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
       <c r="K27" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>575</v>
+        <v>568</v>
       </c>
       <c r="M27" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>687</v>
+        <v>680</v>
       </c>
       <c r="O27" s="3"/>
     </row>
@@ -3740,31 +3740,31 @@
         <v>19</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I28" t="s">
         <v>300</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
       <c r="K28" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="M28" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N28" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O28" s="3"/>
     </row>
@@ -3785,28 +3785,28 @@
         <v>99</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>295</v>
       </c>
       <c r="I29" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="K29" t="s">
         <v>301</v>
       </c>
       <c r="L29" s="5" t="s">
-        <v>640</v>
+        <v>633</v>
       </c>
       <c r="M29" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N29" s="1" t="s">
         <v>100</v>
@@ -3830,10 +3830,10 @@
         <v>56</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="H30" s="7" t="s">
         <v>295</v>
@@ -3842,16 +3842,16 @@
         <v>299</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
       <c r="K30" t="s">
         <v>205</v>
       </c>
       <c r="L30" s="5" t="s">
-        <v>641</v>
+        <v>634</v>
       </c>
       <c r="M30" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N30" s="1" t="s">
         <v>57</v>
@@ -3875,28 +3875,28 @@
         <v>75</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I31" t="s">
         <v>299</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="K31" t="s">
         <v>203</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>565</v>
+        <v>558</v>
       </c>
       <c r="M31" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N31" s="1" t="s">
         <v>76</v>
@@ -3920,28 +3920,28 @@
         <v>126</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I32" t="s">
         <v>299</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="K32" t="s">
         <v>205</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>577</v>
+        <v>570</v>
       </c>
       <c r="M32" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N32" s="1" t="s">
         <v>127</v>
@@ -3965,10 +3965,10 @@
         <v>165</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="H33" s="7" t="s">
         <v>295</v>
@@ -3977,16 +3977,16 @@
         <v>299</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
       <c r="K33" t="s">
         <v>204</v>
       </c>
       <c r="L33" s="5" t="s">
-        <v>642</v>
+        <v>635</v>
       </c>
       <c r="M33" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N33" s="1" t="s">
         <v>166</v>
@@ -4010,10 +4010,10 @@
         <v>172</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="H34" s="7" t="s">
         <v>295</v>
@@ -4022,19 +4022,19 @@
         <v>300</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>562</v>
+        <v>555</v>
       </c>
       <c r="K34" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="M34" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>688</v>
+        <v>681</v>
       </c>
       <c r="O34" s="3"/>
     </row>
@@ -4055,31 +4055,31 @@
         <v>26</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I35" t="s">
         <v>300</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="K35" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>579</v>
+        <v>572</v>
       </c>
       <c r="M35" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>689</v>
+        <v>682</v>
       </c>
       <c r="O35" s="3"/>
     </row>
@@ -4100,28 +4100,28 @@
         <v>77</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I36" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>564</v>
+        <v>557</v>
       </c>
       <c r="K36" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>643</v>
+        <v>636</v>
       </c>
       <c r="M36" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N36" s="1" t="s">
         <v>78</v>
@@ -4145,31 +4145,31 @@
         <v>124</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I37" t="s">
         <v>300</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>565</v>
+        <v>558</v>
       </c>
       <c r="K37" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="L37" s="5" t="s">
-        <v>644</v>
+        <v>637</v>
       </c>
       <c r="M37" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>690</v>
+        <v>683</v>
       </c>
       <c r="O37" s="3"/>
     </row>
@@ -4190,28 +4190,28 @@
         <v>155</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="G38" s="11" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="H38" s="7" t="s">
         <v>295</v>
       </c>
       <c r="I38" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>566</v>
+        <v>559</v>
       </c>
       <c r="K38" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L38" s="5" t="s">
-        <v>645</v>
+        <v>638</v>
       </c>
       <c r="M38" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N38" s="1" t="s">
         <v>156</v>
@@ -4235,28 +4235,28 @@
         <v>63</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="H39" s="7" t="s">
         <v>295</v>
       </c>
       <c r="I39" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>567</v>
+        <v>560</v>
       </c>
       <c r="K39" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="L39" s="5" t="s">
-        <v>646</v>
+        <v>639</v>
       </c>
       <c r="M39" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N39" s="1" t="s">
         <v>64</v>
@@ -4280,28 +4280,28 @@
         <v>179</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="H40" s="7" t="s">
         <v>295</v>
       </c>
       <c r="I40" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>567</v>
+        <v>560</v>
       </c>
       <c r="K40" t="s">
         <v>207</v>
       </c>
       <c r="L40" s="5" t="s">
-        <v>647</v>
+        <v>640</v>
       </c>
       <c r="M40" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N40" s="1" t="s">
         <v>180</v>
@@ -4325,28 +4325,28 @@
         <v>116</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="G41" s="11" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I41" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="K41" t="s">
         <v>207</v>
       </c>
       <c r="L41" s="5" t="s">
-        <v>580</v>
+        <v>573</v>
       </c>
       <c r="M41" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N41" s="1" t="s">
         <v>117</v>
@@ -4370,10 +4370,10 @@
         <v>167</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="G42" s="11" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="H42" s="7" t="s">
         <v>295</v>
@@ -4382,16 +4382,16 @@
         <v>299</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>568</v>
+        <v>561</v>
       </c>
       <c r="K42" t="s">
         <v>204</v>
       </c>
       <c r="L42" s="5" t="s">
-        <v>648</v>
+        <v>641</v>
       </c>
       <c r="M42" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N42" s="1" t="s">
         <v>168</v>
@@ -4415,31 +4415,31 @@
         <v>114</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="H43" s="7" t="s">
         <v>295</v>
       </c>
       <c r="I43" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>569</v>
+        <v>562</v>
       </c>
       <c r="K43" t="s">
         <v>208</v>
       </c>
       <c r="L43" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="M43" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N43" s="10" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="O43" s="3"/>
     </row>
@@ -4460,10 +4460,10 @@
         <v>17</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="G44" s="11" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="H44" s="7" t="s">
         <v>295</v>
@@ -4472,16 +4472,16 @@
         <v>299</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>570</v>
+        <v>563</v>
       </c>
       <c r="K44" t="s">
         <v>203</v>
       </c>
       <c r="L44" s="5" t="s">
-        <v>649</v>
+        <v>642</v>
       </c>
       <c r="M44" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N44" s="1" t="s">
         <v>18</v>
@@ -4505,10 +4505,10 @@
         <v>71</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="H45" s="7" t="s">
         <v>295</v>
@@ -4517,19 +4517,19 @@
         <v>300</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>571</v>
+        <v>564</v>
       </c>
       <c r="K45" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="L45" s="5" t="s">
-        <v>650</v>
+        <v>643</v>
       </c>
       <c r="M45" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N45" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="O45" s="3"/>
     </row>
@@ -4550,28 +4550,28 @@
         <v>32</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I46" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>572</v>
+        <v>565</v>
       </c>
       <c r="K46" t="s">
-        <v>303</v>
+        <v>700</v>
       </c>
       <c r="L46" s="5" t="s">
-        <v>582</v>
+        <v>575</v>
       </c>
       <c r="M46" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N46" s="1" t="s">
         <v>33</v>
@@ -4586,7 +4586,7 @@
         <v>291</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D47" t="s">
         <v>197</v>
@@ -4595,28 +4595,28 @@
         <v>106</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="H47" s="7" t="s">
         <v>295</v>
       </c>
       <c r="I47" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>573</v>
+        <v>566</v>
       </c>
       <c r="K47" t="s">
         <v>208</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>651</v>
+        <v>644</v>
       </c>
       <c r="M47" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N47" s="1" t="s">
         <v>107</v>
@@ -4640,28 +4640,28 @@
         <v>143</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="G48" s="11" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I48" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>574</v>
+        <v>567</v>
       </c>
       <c r="K48" t="s">
         <v>207</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>652</v>
+        <v>645</v>
       </c>
       <c r="M48" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N48" s="1" t="s">
         <v>144</v>
@@ -4685,28 +4685,28 @@
         <v>145</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I49" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>575</v>
+        <v>568</v>
       </c>
       <c r="K49" t="s">
         <v>207</v>
       </c>
       <c r="L49" s="5" t="s">
-        <v>653</v>
+        <v>646</v>
       </c>
       <c r="M49" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N49" s="1" t="s">
         <v>146</v>
@@ -4730,31 +4730,31 @@
         <v>101</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>480</v>
+        <v>473</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I50" t="s">
         <v>300</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>576</v>
+        <v>569</v>
       </c>
       <c r="K50" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>654</v>
+        <v>647</v>
       </c>
       <c r="M50" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>691</v>
+        <v>684</v>
       </c>
       <c r="O50" s="3"/>
     </row>
@@ -4775,31 +4775,31 @@
         <v>105</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="G51" s="11" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
       <c r="H51" s="7" t="s">
         <v>295</v>
       </c>
       <c r="I51" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>577</v>
+        <v>570</v>
       </c>
       <c r="K51" t="s">
         <v>206</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>596</v>
+        <v>589</v>
       </c>
       <c r="M51" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N51" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="O51" s="3"/>
     </row>
@@ -4820,10 +4820,10 @@
         <v>42</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="G52" s="11" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
       <c r="H52" s="7" t="s">
         <v>295</v>
@@ -4832,19 +4832,19 @@
         <v>300</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>578</v>
+        <v>571</v>
       </c>
       <c r="K52" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L52" s="5" t="s">
-        <v>652</v>
+        <v>645</v>
       </c>
       <c r="M52" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N52" s="9" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="O52" s="3"/>
     </row>
@@ -4865,28 +4865,28 @@
         <v>185</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="G53" s="11" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
       <c r="H53" s="7" t="s">
         <v>295</v>
       </c>
       <c r="I53" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>578</v>
+        <v>571</v>
       </c>
       <c r="K53" t="s">
         <v>206</v>
       </c>
       <c r="L53" s="5" t="s">
-        <v>601</v>
+        <v>594</v>
       </c>
       <c r="M53" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N53" s="1" t="s">
         <v>186</v>
@@ -4910,10 +4910,10 @@
         <v>82</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="G54" s="11" t="s">
-        <v>484</v>
+        <v>477</v>
       </c>
       <c r="H54" s="7" t="s">
         <v>295</v>
@@ -4922,16 +4922,16 @@
         <v>299</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>579</v>
+        <v>572</v>
       </c>
       <c r="K54" t="s">
         <v>204</v>
       </c>
       <c r="L54" s="5" t="s">
-        <v>655</v>
+        <v>648</v>
       </c>
       <c r="M54" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N54" s="1" t="s">
         <v>83</v>
@@ -4946,7 +4946,7 @@
         <v>291</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D55" t="s">
         <v>199</v>
@@ -4955,31 +4955,31 @@
         <v>171</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>347</v>
+        <v>695</v>
       </c>
       <c r="G55" s="11" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I55" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>580</v>
+        <v>573</v>
       </c>
       <c r="K55" t="s">
-        <v>303</v>
+        <v>700</v>
       </c>
       <c r="L55" s="5" t="s">
-        <v>656</v>
+        <v>649</v>
       </c>
       <c r="M55" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="N55" s="1" t="s">
-        <v>692</v>
+        <v>685</v>
       </c>
       <c r="O55" s="3"/>
     </row>
@@ -4991,7 +4991,7 @@
         <v>284</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D56" t="s">
         <v>197</v>
@@ -5000,10 +5000,10 @@
         <v>108</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="G56" s="11" t="s">
-        <v>486</v>
+        <v>479</v>
       </c>
       <c r="H56" s="7" t="s">
         <v>295</v>
@@ -5012,16 +5012,16 @@
         <v>299</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>581</v>
+        <v>574</v>
       </c>
       <c r="K56" t="s">
         <v>204</v>
       </c>
       <c r="L56" s="5" t="s">
-        <v>585</v>
+        <v>578</v>
       </c>
       <c r="M56" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N56" s="1" t="s">
         <v>109</v>
@@ -5045,28 +5045,28 @@
         <v>183</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="G57" s="11" t="s">
-        <v>487</v>
+        <v>480</v>
       </c>
       <c r="H57" s="7" t="s">
         <v>295</v>
       </c>
       <c r="I57" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>582</v>
+        <v>575</v>
       </c>
       <c r="K57" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L57" s="5" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
       <c r="M57" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N57" s="1" t="s">
         <v>184</v>
@@ -5090,28 +5090,28 @@
         <v>93</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>488</v>
+        <v>481</v>
       </c>
       <c r="H58" s="7" t="s">
         <v>295</v>
       </c>
       <c r="I58" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>583</v>
+        <v>576</v>
       </c>
       <c r="K58" t="s">
         <v>302</v>
       </c>
       <c r="L58" s="5" t="s">
-        <v>658</v>
+        <v>651</v>
       </c>
       <c r="M58" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N58" s="1" t="s">
         <v>94</v>
@@ -5135,28 +5135,28 @@
         <v>45</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="G59" s="11" t="s">
-        <v>489</v>
+        <v>482</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I59" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>584</v>
+        <v>577</v>
       </c>
       <c r="K59" t="s">
         <v>301</v>
       </c>
       <c r="L59" s="5" t="s">
-        <v>584</v>
+        <v>577</v>
       </c>
       <c r="M59" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N59" s="1" t="s">
         <v>46</v>
@@ -5180,28 +5180,28 @@
         <v>34</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="G60" s="11" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
       <c r="H60" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I60" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>584</v>
+        <v>577</v>
       </c>
       <c r="K60" t="s">
         <v>206</v>
       </c>
       <c r="L60" s="5" t="s">
-        <v>601</v>
+        <v>594</v>
       </c>
       <c r="M60" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N60" s="1" t="s">
         <v>35</v>
@@ -5225,28 +5225,28 @@
         <v>14</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="G61" s="11" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="H61" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I61" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>585</v>
+        <v>578</v>
       </c>
       <c r="K61" t="s">
         <v>207</v>
       </c>
       <c r="L61" s="5" t="s">
-        <v>659</v>
+        <v>652</v>
       </c>
       <c r="M61" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N61" s="1" t="s">
         <v>15</v>
@@ -5270,28 +5270,28 @@
         <v>138</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="G62" s="11" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
       <c r="H62" s="7" t="s">
         <v>295</v>
       </c>
       <c r="I62" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="J62" s="5" t="s">
-        <v>585</v>
+        <v>578</v>
       </c>
       <c r="K62" t="s">
         <v>207</v>
       </c>
       <c r="L62" s="5" t="s">
-        <v>660</v>
+        <v>653</v>
       </c>
       <c r="M62" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N62" s="1" t="s">
         <v>139</v>
@@ -5315,28 +5315,28 @@
         <v>38</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>335</v>
+        <v>696</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="H63" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I63" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="J63" s="5" t="s">
-        <v>586</v>
+        <v>579</v>
       </c>
       <c r="K63" t="s">
         <v>302</v>
       </c>
       <c r="L63" s="5" t="s">
-        <v>661</v>
+        <v>654</v>
       </c>
       <c r="M63" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N63" s="1" t="s">
         <v>39</v>
@@ -5360,28 +5360,28 @@
         <v>159</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="G64" s="11" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="H64" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I64" t="s">
         <v>299</v>
       </c>
       <c r="J64" s="5" t="s">
-        <v>587</v>
+        <v>580</v>
       </c>
       <c r="K64" t="s">
         <v>204</v>
       </c>
       <c r="L64" s="5" t="s">
-        <v>662</v>
+        <v>655</v>
       </c>
       <c r="M64" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N64" s="1" t="s">
         <v>160</v>
@@ -5405,10 +5405,10 @@
         <v>123</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>346</v>
+        <v>697</v>
       </c>
       <c r="G65" s="11" t="s">
-        <v>495</v>
+        <v>488</v>
       </c>
       <c r="H65" s="7" t="s">
         <v>295</v>
@@ -5417,19 +5417,19 @@
         <v>300</v>
       </c>
       <c r="J65" s="5" t="s">
-        <v>588</v>
+        <v>581</v>
       </c>
       <c r="K65" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L65" s="5" t="s">
-        <v>663</v>
+        <v>656</v>
       </c>
       <c r="M65" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N65" s="1" t="s">
-        <v>693</v>
+        <v>686</v>
       </c>
       <c r="O65" s="3"/>
     </row>
@@ -5450,10 +5450,10 @@
         <v>189</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="G66" s="11" t="s">
-        <v>496</v>
+        <v>489</v>
       </c>
       <c r="H66" s="7" t="s">
         <v>295</v>
@@ -5462,19 +5462,19 @@
         <v>300</v>
       </c>
       <c r="J66" s="5" t="s">
-        <v>589</v>
+        <v>582</v>
       </c>
       <c r="K66" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L66" s="5" t="s">
-        <v>664</v>
+        <v>657</v>
       </c>
       <c r="M66" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N66" s="1" t="s">
-        <v>694</v>
+        <v>687</v>
       </c>
       <c r="O66" s="3"/>
     </row>
@@ -5495,28 +5495,28 @@
         <v>28</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="G67" s="11" t="s">
-        <v>497</v>
+        <v>490</v>
       </c>
       <c r="H67" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I67" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="J67" s="5" t="s">
-        <v>590</v>
+        <v>583</v>
       </c>
       <c r="K67" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="L67" s="5" t="s">
-        <v>665</v>
+        <v>658</v>
       </c>
       <c r="M67" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N67" s="1" t="s">
         <v>29</v>
@@ -5540,28 +5540,28 @@
         <v>52</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="G68" s="11" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
       <c r="H68" s="7" t="s">
         <v>295</v>
       </c>
       <c r="I68" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="J68" s="5" t="s">
-        <v>591</v>
+        <v>584</v>
       </c>
       <c r="K68" t="s">
         <v>208</v>
       </c>
       <c r="L68" s="5" t="s">
-        <v>666</v>
+        <v>659</v>
       </c>
       <c r="M68" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N68" s="1" t="s">
         <v>53</v>
@@ -5585,28 +5585,28 @@
         <v>68</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="G69" s="11" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
       <c r="H69" s="7" t="s">
         <v>295</v>
       </c>
       <c r="I69" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="J69" s="5" t="s">
-        <v>592</v>
+        <v>585</v>
       </c>
       <c r="K69" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="L69" s="5" t="s">
-        <v>667</v>
+        <v>660</v>
       </c>
       <c r="M69" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N69" s="1" t="s">
         <v>69</v>
@@ -5630,10 +5630,10 @@
         <v>10</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="G70" s="11" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
       <c r="H70" s="7" t="s">
         <v>295</v>
@@ -5642,16 +5642,16 @@
         <v>299</v>
       </c>
       <c r="J70" s="5" t="s">
-        <v>593</v>
+        <v>586</v>
       </c>
       <c r="K70" t="s">
         <v>205</v>
       </c>
       <c r="L70" s="5" t="s">
-        <v>668</v>
+        <v>661</v>
       </c>
       <c r="M70" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N70" s="1" t="s">
         <v>11</v>
@@ -5675,28 +5675,28 @@
         <v>91</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G71" s="11" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
       <c r="H71" s="7" t="s">
         <v>295</v>
       </c>
       <c r="I71" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="J71" s="5" t="s">
-        <v>594</v>
+        <v>587</v>
       </c>
       <c r="K71" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="L71" s="5" t="s">
-        <v>669</v>
+        <v>662</v>
       </c>
       <c r="M71" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N71" s="1" t="s">
         <v>92</v>
@@ -5720,28 +5720,28 @@
         <v>110</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="G72" s="11" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
       <c r="H72" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I72" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="J72" s="5" t="s">
-        <v>594</v>
+        <v>587</v>
       </c>
       <c r="K72" t="s">
         <v>208</v>
       </c>
       <c r="L72" s="5" t="s">
-        <v>670</v>
+        <v>663</v>
       </c>
       <c r="M72" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N72" s="1" t="s">
         <v>111</v>
@@ -5765,28 +5765,28 @@
         <v>119</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="G73" s="11" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
       <c r="H73" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I73" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="J73" s="5" t="s">
-        <v>594</v>
+        <v>587</v>
       </c>
       <c r="K73" t="s">
         <v>207</v>
       </c>
       <c r="L73" s="5" t="s">
-        <v>671</v>
+        <v>664</v>
       </c>
       <c r="M73" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N73" s="1" t="s">
         <v>120</v>
@@ -5810,10 +5810,10 @@
         <v>104</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="G74" s="12" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
       <c r="H74" s="7" t="s">
         <v>295</v>
@@ -5822,19 +5822,19 @@
         <v>300</v>
       </c>
       <c r="J74" s="5" t="s">
-        <v>595</v>
+        <v>588</v>
       </c>
       <c r="K74" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L74" s="5" t="s">
-        <v>612</v>
+        <v>605</v>
       </c>
       <c r="M74" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N74" s="1" t="s">
-        <v>695</v>
+        <v>688</v>
       </c>
       <c r="O74" s="3"/>
     </row>
@@ -5855,28 +5855,28 @@
         <v>22</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="G75" s="11" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
       <c r="H75" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I75" t="s">
         <v>299</v>
       </c>
       <c r="J75" s="5" t="s">
-        <v>596</v>
+        <v>589</v>
       </c>
       <c r="K75" t="s">
         <v>203</v>
       </c>
       <c r="L75" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="M75" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N75" s="1" t="s">
         <v>23</v>
@@ -5900,28 +5900,28 @@
         <v>147</v>
       </c>
       <c r="F76" s="7" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G76" s="11" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="H76" s="7" t="s">
         <v>295</v>
       </c>
       <c r="I76" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="J76" s="5" t="s">
-        <v>597</v>
+        <v>590</v>
       </c>
       <c r="K76" t="s">
         <v>206</v>
       </c>
       <c r="L76" s="5" t="s">
-        <v>670</v>
+        <v>663</v>
       </c>
       <c r="M76" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N76" s="1" t="s">
         <v>148</v>
@@ -5945,28 +5945,28 @@
         <v>153</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G77" s="11" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="H77" s="7" t="s">
         <v>295</v>
       </c>
       <c r="I77" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="J77" s="5" t="s">
-        <v>598</v>
+        <v>591</v>
       </c>
       <c r="K77" t="s">
         <v>207</v>
       </c>
       <c r="L77" s="5" t="s">
-        <v>666</v>
+        <v>659</v>
       </c>
       <c r="M77" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N77" s="1" t="s">
         <v>154</v>
@@ -5990,28 +5990,28 @@
         <v>8</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>409</v>
+        <v>698</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="H78" s="7" t="s">
         <v>295</v>
       </c>
       <c r="I78" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="J78" s="5" t="s">
-        <v>599</v>
+        <v>592</v>
       </c>
       <c r="K78" t="s">
         <v>207</v>
       </c>
       <c r="L78" s="5" t="s">
-        <v>672</v>
+        <v>665</v>
       </c>
       <c r="M78" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N78" s="1" t="s">
         <v>9</v>
@@ -6035,28 +6035,28 @@
         <v>136</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="G79" s="11" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
       <c r="H79" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I79" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="J79" s="5" t="s">
-        <v>600</v>
+        <v>593</v>
       </c>
       <c r="K79" t="s">
         <v>301</v>
       </c>
       <c r="L79" s="5" t="s">
-        <v>609</v>
+        <v>602</v>
       </c>
       <c r="M79" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N79" s="1" t="s">
         <v>137</v>
@@ -6080,10 +6080,10 @@
         <v>152</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="G80" s="12" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="H80" s="7" t="s">
         <v>295</v>
@@ -6092,19 +6092,19 @@
         <v>300</v>
       </c>
       <c r="J80" s="5" t="s">
-        <v>601</v>
+        <v>594</v>
       </c>
       <c r="K80" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="L80" s="5" t="s">
-        <v>673</v>
+        <v>666</v>
       </c>
       <c r="M80" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N80" s="1" t="s">
-        <v>696</v>
+        <v>689</v>
       </c>
       <c r="O80" s="3"/>
     </row>
@@ -6125,28 +6125,28 @@
         <v>179</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="G81" s="11" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
       <c r="H81" s="7" t="s">
         <v>295</v>
       </c>
       <c r="I81" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="J81" s="5" t="s">
-        <v>602</v>
+        <v>595</v>
       </c>
       <c r="K81" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="L81" s="5" t="s">
-        <v>674</v>
+        <v>667</v>
       </c>
       <c r="M81" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N81" s="1" t="s">
         <v>180</v>
@@ -6170,28 +6170,28 @@
         <v>89</v>
       </c>
       <c r="F82" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G82" s="11" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
       <c r="H82" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I82" t="s">
         <v>299</v>
       </c>
       <c r="J82" s="5" t="s">
-        <v>603</v>
+        <v>596</v>
       </c>
       <c r="K82" t="s">
         <v>204</v>
       </c>
       <c r="L82" s="5" t="s">
-        <v>675</v>
+        <v>668</v>
       </c>
       <c r="M82" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N82" s="1" t="s">
         <v>90</v>
@@ -6215,28 +6215,28 @@
         <v>65</v>
       </c>
       <c r="F83" s="7" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="G83" s="11" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
       <c r="H83" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I83" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="J83" s="5" t="s">
-        <v>604</v>
+        <v>597</v>
       </c>
       <c r="K83" t="s">
         <v>302</v>
       </c>
       <c r="L83" s="5" t="s">
-        <v>676</v>
+        <v>669</v>
       </c>
       <c r="M83" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N83" s="1" t="s">
         <v>66</v>
@@ -6260,28 +6260,28 @@
         <v>121</v>
       </c>
       <c r="F84" s="7" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="G84" s="11" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
       <c r="H84" s="7" t="s">
         <v>295</v>
       </c>
       <c r="I84" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="J84" s="5" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
       <c r="K84" t="s">
         <v>207</v>
       </c>
       <c r="L84" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="M84" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N84" s="1" t="s">
         <v>122</v>
@@ -6305,28 +6305,28 @@
         <v>175</v>
       </c>
       <c r="F85" s="7" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="G85" s="11" t="s">
-        <v>514</v>
+        <v>507</v>
       </c>
       <c r="H85" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I85" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="J85" s="5" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
       <c r="K85" t="s">
-        <v>303</v>
+        <v>700</v>
       </c>
       <c r="L85" s="5" t="s">
-        <v>677</v>
+        <v>670</v>
       </c>
       <c r="M85" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N85" s="1" t="s">
         <v>176</v>
@@ -6350,10 +6350,10 @@
         <v>97</v>
       </c>
       <c r="F86" s="7" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="G86" s="11" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
       <c r="H86" s="7" t="s">
         <v>295</v>
@@ -6362,16 +6362,16 @@
         <v>299</v>
       </c>
       <c r="J86" s="5" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="K86" t="s">
         <v>204</v>
       </c>
       <c r="L86" s="5" t="s">
-        <v>614</v>
+        <v>607</v>
       </c>
       <c r="M86" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N86" s="1" t="s">
         <v>98</v>
@@ -6395,28 +6395,28 @@
         <v>140</v>
       </c>
       <c r="F87" s="7" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="G87" s="11" t="s">
-        <v>516</v>
+        <v>509</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I87" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="J87" s="5" t="s">
-        <v>607</v>
+        <v>600</v>
       </c>
       <c r="K87" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="L87" s="5" t="s">
-        <v>678</v>
+        <v>671</v>
       </c>
       <c r="M87" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N87" s="1" t="s">
         <v>141</v>
@@ -6440,31 +6440,31 @@
         <v>174</v>
       </c>
       <c r="F88" s="7" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="G88" s="12" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
       <c r="H88" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I88" t="s">
         <v>300</v>
       </c>
       <c r="J88" s="5" t="s">
-        <v>608</v>
+        <v>601</v>
       </c>
       <c r="K88" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L88" s="5" t="s">
-        <v>678</v>
+        <v>671</v>
       </c>
       <c r="M88" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N88" s="1" t="s">
-        <v>697</v>
+        <v>690</v>
       </c>
       <c r="O88" s="3"/>
     </row>
@@ -6485,31 +6485,31 @@
         <v>27</v>
       </c>
       <c r="F89" s="7" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="G89" s="11" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
       <c r="H89" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I89" t="s">
         <v>300</v>
       </c>
       <c r="J89" s="5" t="s">
-        <v>609</v>
+        <v>602</v>
       </c>
       <c r="K89" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="L89" s="5" t="s">
-        <v>612</v>
+        <v>605</v>
       </c>
       <c r="M89" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N89" s="1" t="s">
-        <v>698</v>
+        <v>691</v>
       </c>
       <c r="O89" s="3"/>
     </row>
@@ -6530,28 +6530,28 @@
         <v>12</v>
       </c>
       <c r="F90" s="7" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="G90" s="11" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
       <c r="H90" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I90" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="J90" s="5" t="s">
-        <v>610</v>
+        <v>603</v>
       </c>
       <c r="K90" t="s">
         <v>208</v>
       </c>
       <c r="L90" s="5" t="s">
-        <v>679</v>
+        <v>672</v>
       </c>
       <c r="M90" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N90" s="1" t="s">
         <v>13</v>
@@ -6575,28 +6575,28 @@
         <v>43</v>
       </c>
       <c r="F91" s="7" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="G91" s="11" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
       <c r="H91" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I91" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="J91" s="5" t="s">
-        <v>611</v>
+        <v>604</v>
       </c>
       <c r="K91" t="s">
         <v>208</v>
       </c>
       <c r="L91" s="5" t="s">
-        <v>680</v>
+        <v>673</v>
       </c>
       <c r="M91" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N91" s="1" t="s">
         <v>44</v>
@@ -6620,31 +6620,31 @@
         <v>118</v>
       </c>
       <c r="F92" s="7" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="G92" s="11" t="s">
-        <v>521</v>
+        <v>514</v>
       </c>
       <c r="H92" s="8" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="I92" t="s">
         <v>300</v>
       </c>
       <c r="J92" s="5" t="s">
-        <v>612</v>
+        <v>605</v>
       </c>
       <c r="K92" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L92" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="M92" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N92" s="1" t="s">
-        <v>699</v>
+        <v>692</v>
       </c>
       <c r="O92" s="3"/>
     </row>
@@ -6665,10 +6665,10 @@
         <v>61</v>
       </c>
       <c r="F93" s="7" t="s">
-        <v>345</v>
+        <v>699</v>
       </c>
       <c r="G93" s="11" t="s">
-        <v>522</v>
+        <v>515</v>
       </c>
       <c r="H93" s="7" t="s">
         <v>295</v>
@@ -6677,16 +6677,16 @@
         <v>299</v>
       </c>
       <c r="J93" s="5" t="s">
-        <v>612</v>
+        <v>605</v>
       </c>
       <c r="K93" t="s">
         <v>203</v>
       </c>
       <c r="L93" s="5" t="s">
-        <v>678</v>
+        <v>671</v>
       </c>
       <c r="M93" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N93" s="1" t="s">
         <v>62</v>
@@ -6710,31 +6710,31 @@
         <v>24</v>
       </c>
       <c r="F94" s="7" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="G94" s="11" t="s">
-        <v>523</v>
+        <v>516</v>
       </c>
       <c r="H94" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I94" t="s">
         <v>300</v>
       </c>
       <c r="J94" s="5" t="s">
-        <v>613</v>
+        <v>606</v>
       </c>
       <c r="K94" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L94" s="5" t="s">
-        <v>681</v>
+        <v>674</v>
       </c>
       <c r="M94" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N94" s="1" t="s">
-        <v>700</v>
+        <v>693</v>
       </c>
       <c r="O94" s="3"/>
     </row>
@@ -6755,28 +6755,28 @@
         <v>161</v>
       </c>
       <c r="F95" s="7" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="G95" s="11" t="s">
+        <v>517</v>
+      </c>
+      <c r="H95" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="I95" t="s">
         <v>524</v>
       </c>
-      <c r="H95" s="7" t="s">
-        <v>328</v>
-      </c>
-      <c r="I95" t="s">
-        <v>531</v>
-      </c>
       <c r="J95" s="5" t="s">
-        <v>614</v>
+        <v>607</v>
       </c>
       <c r="K95" t="s">
         <v>208</v>
       </c>
       <c r="L95" s="5" t="s">
-        <v>614</v>
+        <v>607</v>
       </c>
       <c r="M95" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N95" s="1" t="s">
         <v>162</v>
@@ -6800,31 +6800,31 @@
         <v>171</v>
       </c>
       <c r="F96" s="7" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="G96" s="11" t="s">
-        <v>525</v>
+        <v>518</v>
       </c>
       <c r="H96" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I96" t="s">
         <v>300</v>
       </c>
       <c r="J96" s="5" t="s">
-        <v>615</v>
+        <v>608</v>
       </c>
       <c r="K96" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L96" s="5" t="s">
-        <v>639</v>
+        <v>632</v>
       </c>
       <c r="M96" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N96" s="1" t="s">
-        <v>692</v>
+        <v>685</v>
       </c>
       <c r="O96" s="3"/>
     </row>
@@ -6845,28 +6845,28 @@
         <v>112</v>
       </c>
       <c r="F97" s="7" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="G97" s="11" t="s">
-        <v>526</v>
+        <v>519</v>
       </c>
       <c r="H97" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I97" t="s">
         <v>299</v>
       </c>
       <c r="J97" s="5" t="s">
-        <v>616</v>
+        <v>609</v>
       </c>
       <c r="K97" t="s">
         <v>205</v>
       </c>
       <c r="L97" s="5" t="s">
-        <v>682</v>
+        <v>675</v>
       </c>
       <c r="M97" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N97" s="1" t="s">
         <v>113</v>
@@ -6890,28 +6890,28 @@
         <v>187</v>
       </c>
       <c r="F98" s="7" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="G98" s="11" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="H98" s="7" t="s">
         <v>295</v>
       </c>
       <c r="I98" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="J98" s="5" t="s">
-        <v>617</v>
+        <v>610</v>
       </c>
       <c r="K98" t="s">
         <v>207</v>
       </c>
       <c r="L98" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="M98" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N98" s="1" t="s">
         <v>188</v>
@@ -6935,28 +6935,28 @@
         <v>130</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="G99" s="11" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
       <c r="H99" s="7" t="s">
         <v>295</v>
       </c>
       <c r="I99" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="J99" s="5" t="s">
-        <v>618</v>
+        <v>611</v>
       </c>
       <c r="K99" t="s">
         <v>301</v>
       </c>
       <c r="L99" s="5" t="s">
-        <v>674</v>
+        <v>667</v>
       </c>
       <c r="M99" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N99" s="1" t="s">
         <v>131</v>
@@ -6980,31 +6980,31 @@
         <v>103</v>
       </c>
       <c r="F100" s="7" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="G100" s="11" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="H100" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I100" t="s">
         <v>299</v>
       </c>
       <c r="J100" s="5" t="s">
-        <v>619</v>
+        <v>612</v>
       </c>
       <c r="K100" t="s">
         <v>203</v>
       </c>
       <c r="L100" s="5" t="s">
-        <v>682</v>
+        <v>675</v>
       </c>
       <c r="M100" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N100" s="10" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="O100" s="3"/>
     </row>
@@ -7025,28 +7025,28 @@
         <v>85</v>
       </c>
       <c r="F101" s="7" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="G101" s="11" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
       <c r="H101" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I101" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="J101" s="5" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
       <c r="K101" t="s">
         <v>301</v>
       </c>
       <c r="L101" s="5" t="s">
-        <v>683</v>
+        <v>676</v>
       </c>
       <c r="M101" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N101" s="1" t="s">
         <v>86</v>

</xml_diff>

<commit_message>
Data Columns Split in their Respected Tables
Patient, Referrer, Surgeon, Referral
</commit_message>
<xml_diff>
--- a/ARA DATA Wait Lists Feb 2021.xlsx
+++ b/ARA DATA Wait Lists Feb 2021.xlsx
@@ -1,24 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tewaka-my.sharepoint.com/personal/jra0108_arastudent_ac_nz/Documents/2021/Bachelor (Sem2)/BCDE103/Assessment/Assignment 1/Submit/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tewaka-my.sharepoint.com/personal/jra0108_arastudent_ac_nz/Documents/2021/Bachelor (Sem2)/BCDE103/Assessment/Assignment 1/Submit/Iteration1/Data Cleansing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="336" documentId="13_ncr:1_{F62C6F57-4F11-4DC1-8AB4-9BAEA44BD995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC63218C-5FD3-4A18-9097-92C92445C0BF}"/>
+  <xr:revisionPtr revIDLastSave="498" documentId="13_ncr:1_{F62C6F57-4F11-4DC1-8AB4-9BAEA44BD995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{758FD868-3AB2-451A-8BDE-7CAD27E49412}"/>
   <bookViews>
-    <workbookView xWindow="1725" yWindow="5760" windowWidth="25365" windowHeight="13635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="705" yWindow="2865" windowWidth="22170" windowHeight="17970" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" state="hidden" r:id="rId3"/>
+    <sheet name="Patient" sheetId="4" r:id="rId2"/>
+    <sheet name="Referrer" sheetId="5" r:id="rId3"/>
+    <sheet name="Surgeon" sheetId="6" r:id="rId4"/>
+    <sheet name="Referral" sheetId="7" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="3" state="hidden" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet2!$A$1:$A$2330</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Sheet2!$A$1:$A$2330</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Worksheet!$A$1:$T$101</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1403" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2016" uniqueCount="486">
   <si>
     <t>Referral Date</t>
   </si>
@@ -1480,6 +1483,21 @@
   </si>
   <si>
     <t>Referrer Last Name</t>
+  </si>
+  <si>
+    <t>patientNumber</t>
+  </si>
+  <si>
+    <t>Staff ID</t>
+  </si>
+  <si>
+    <t>Referrer Code</t>
+  </si>
+  <si>
+    <t>Referral Code</t>
+  </si>
+  <si>
+    <t>Patient Number</t>
   </si>
 </sst>
 </file>
@@ -1522,7 +1540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFill="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
@@ -1530,6 +1548,8 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1812,8 +1832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R106" sqref="R106"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K56" sqref="K56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7507,20 +7527,4894 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A100"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" t="s">
+        <v>251</v>
+      </c>
+      <c r="D2" t="s">
+        <v>252</v>
+      </c>
+      <c r="E2" s="3">
+        <v>26343</v>
+      </c>
+      <c r="F2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s">
+        <v>253</v>
+      </c>
+      <c r="D3" t="s">
+        <v>449</v>
+      </c>
+      <c r="E3" s="3">
+        <v>33965</v>
+      </c>
+      <c r="F3" t="s">
+        <v>220</v>
+      </c>
+      <c r="G3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D4" t="s">
+        <v>255</v>
+      </c>
+      <c r="E4" s="3">
+        <v>18737</v>
+      </c>
+      <c r="F4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" t="s">
+        <v>256</v>
+      </c>
+      <c r="D5" t="s">
+        <v>257</v>
+      </c>
+      <c r="E5" s="3">
+        <v>22765</v>
+      </c>
+      <c r="F5" t="s">
+        <v>189</v>
+      </c>
+      <c r="G5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" t="s">
+        <v>258</v>
+      </c>
+      <c r="D6" t="s">
+        <v>259</v>
+      </c>
+      <c r="E6" s="3">
+        <v>32802</v>
+      </c>
+      <c r="F6" t="s">
+        <v>220</v>
+      </c>
+      <c r="G6" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" t="s">
+        <v>260</v>
+      </c>
+      <c r="D7" t="s">
+        <v>261</v>
+      </c>
+      <c r="E7" s="3">
+        <v>23786</v>
+      </c>
+      <c r="F7" t="s">
+        <v>189</v>
+      </c>
+      <c r="G7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" t="s">
+        <v>262</v>
+      </c>
+      <c r="D8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E8" s="3">
+        <v>24871</v>
+      </c>
+      <c r="F8" t="s">
+        <v>220</v>
+      </c>
+      <c r="G8" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" t="s">
+        <v>264</v>
+      </c>
+      <c r="D9" t="s">
+        <v>265</v>
+      </c>
+      <c r="E9" s="3">
+        <v>17827</v>
+      </c>
+      <c r="F9" t="s">
+        <v>189</v>
+      </c>
+      <c r="G9" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>266</v>
+      </c>
+      <c r="D10" t="s">
+        <v>267</v>
+      </c>
+      <c r="E10" s="3">
+        <v>27605</v>
+      </c>
+      <c r="F10" t="s">
+        <v>189</v>
+      </c>
+      <c r="G10" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" t="s">
+        <v>268</v>
+      </c>
+      <c r="D11" t="s">
+        <v>269</v>
+      </c>
+      <c r="E11" s="3">
+        <v>39645</v>
+      </c>
+      <c r="F11" t="s">
+        <v>189</v>
+      </c>
+      <c r="G11" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" t="s">
+        <v>270</v>
+      </c>
+      <c r="D12" t="s">
+        <v>271</v>
+      </c>
+      <c r="E12" s="3">
+        <v>38646</v>
+      </c>
+      <c r="F12" t="s">
+        <v>220</v>
+      </c>
+      <c r="G12" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>138</v>
+      </c>
+      <c r="C13" t="s">
+        <v>272</v>
+      </c>
+      <c r="D13" t="s">
+        <v>273</v>
+      </c>
+      <c r="E13" s="3">
+        <v>20984</v>
+      </c>
+      <c r="F13" t="s">
+        <v>220</v>
+      </c>
+      <c r="G13" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>160</v>
+      </c>
+      <c r="C14" t="s">
+        <v>274</v>
+      </c>
+      <c r="D14" t="s">
+        <v>275</v>
+      </c>
+      <c r="E14" s="3">
+        <v>29458</v>
+      </c>
+      <c r="F14" t="s">
+        <v>220</v>
+      </c>
+      <c r="G14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" t="s">
+        <v>276</v>
+      </c>
+      <c r="D15" t="s">
+        <v>277</v>
+      </c>
+      <c r="E15" s="3">
+        <v>41392</v>
+      </c>
+      <c r="F15" t="s">
+        <v>189</v>
+      </c>
+      <c r="G15" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C16" t="s">
+        <v>278</v>
+      </c>
+      <c r="D16" t="s">
+        <v>279</v>
+      </c>
+      <c r="E16" s="3">
+        <v>27857</v>
+      </c>
+      <c r="F16" t="s">
+        <v>189</v>
+      </c>
+      <c r="G16" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
+        <v>280</v>
+      </c>
+      <c r="D17" t="s">
+        <v>281</v>
+      </c>
+      <c r="E17" s="3">
+        <v>41785</v>
+      </c>
+      <c r="F17" t="s">
+        <v>220</v>
+      </c>
+      <c r="G17" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>282</v>
+      </c>
+      <c r="D18" t="s">
+        <v>283</v>
+      </c>
+      <c r="E18" s="3">
+        <v>22327</v>
+      </c>
+      <c r="F18" t="s">
+        <v>189</v>
+      </c>
+      <c r="G18" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>116</v>
+      </c>
+      <c r="C19" t="s">
+        <v>284</v>
+      </c>
+      <c r="D19" t="s">
+        <v>285</v>
+      </c>
+      <c r="E19" s="3">
+        <v>42375</v>
+      </c>
+      <c r="F19" t="s">
+        <v>220</v>
+      </c>
+      <c r="G19" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
+        <v>286</v>
+      </c>
+      <c r="D20" t="s">
+        <v>287</v>
+      </c>
+      <c r="E20" s="3">
+        <v>24627</v>
+      </c>
+      <c r="F20" t="s">
+        <v>220</v>
+      </c>
+      <c r="G20" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>288</v>
+      </c>
+      <c r="D21" t="s">
+        <v>289</v>
+      </c>
+      <c r="E21" s="3">
+        <v>24573</v>
+      </c>
+      <c r="F21" t="s">
+        <v>189</v>
+      </c>
+      <c r="G21" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>167</v>
+      </c>
+      <c r="C22" t="s">
+        <v>290</v>
+      </c>
+      <c r="D22" t="s">
+        <v>291</v>
+      </c>
+      <c r="E22" s="3">
+        <v>28403</v>
+      </c>
+      <c r="F22" t="s">
+        <v>220</v>
+      </c>
+      <c r="G22" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" t="s">
+        <v>292</v>
+      </c>
+      <c r="D23" t="s">
+        <v>293</v>
+      </c>
+      <c r="E23" s="3">
+        <v>37966</v>
+      </c>
+      <c r="F23" t="s">
+        <v>222</v>
+      </c>
+      <c r="G23" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
+        <v>294</v>
+      </c>
+      <c r="D24" t="s">
+        <v>295</v>
+      </c>
+      <c r="E24" s="3">
+        <v>30916</v>
+      </c>
+      <c r="F24" t="s">
+        <v>189</v>
+      </c>
+      <c r="G24" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" t="s">
+        <v>296</v>
+      </c>
+      <c r="D25" t="s">
+        <v>297</v>
+      </c>
+      <c r="E25" s="3">
+        <v>38973</v>
+      </c>
+      <c r="F25" t="s">
+        <v>189</v>
+      </c>
+      <c r="G25" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" t="s">
+        <v>298</v>
+      </c>
+      <c r="D26" t="s">
+        <v>299</v>
+      </c>
+      <c r="E26" s="3">
+        <v>19044</v>
+      </c>
+      <c r="F26" t="s">
+        <v>220</v>
+      </c>
+      <c r="G26" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" t="s">
+        <v>300</v>
+      </c>
+      <c r="D27" t="s">
+        <v>301</v>
+      </c>
+      <c r="E27" s="3">
+        <v>40516</v>
+      </c>
+      <c r="F27" t="s">
+        <v>220</v>
+      </c>
+      <c r="G27" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" t="s">
+        <v>302</v>
+      </c>
+      <c r="D28" t="s">
+        <v>303</v>
+      </c>
+      <c r="E28" s="3">
+        <v>41266</v>
+      </c>
+      <c r="F28" t="s">
+        <v>220</v>
+      </c>
+      <c r="G28" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" t="s">
+        <v>304</v>
+      </c>
+      <c r="D29" t="s">
+        <v>305</v>
+      </c>
+      <c r="E29" s="3">
+        <v>40305</v>
+      </c>
+      <c r="F29" t="s">
+        <v>189</v>
+      </c>
+      <c r="G29" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" t="s">
+        <v>306</v>
+      </c>
+      <c r="D30" t="s">
+        <v>307</v>
+      </c>
+      <c r="E30" s="3">
+        <v>19036</v>
+      </c>
+      <c r="F30" t="s">
+        <v>189</v>
+      </c>
+      <c r="G30" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" t="s">
+        <v>308</v>
+      </c>
+      <c r="D31" t="s">
+        <v>309</v>
+      </c>
+      <c r="E31" s="3">
+        <v>23051</v>
+      </c>
+      <c r="F31" t="s">
+        <v>220</v>
+      </c>
+      <c r="G31" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>111</v>
+      </c>
+      <c r="C32" t="s">
+        <v>310</v>
+      </c>
+      <c r="D32" t="s">
+        <v>311</v>
+      </c>
+      <c r="E32" s="3">
+        <v>23935</v>
+      </c>
+      <c r="F32" t="s">
+        <v>220</v>
+      </c>
+      <c r="G32" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>145</v>
+      </c>
+      <c r="C33" t="s">
+        <v>312</v>
+      </c>
+      <c r="D33" t="s">
+        <v>313</v>
+      </c>
+      <c r="E33" s="3">
+        <v>31929</v>
+      </c>
+      <c r="F33" t="s">
+        <v>189</v>
+      </c>
+      <c r="G33" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>152</v>
+      </c>
+      <c r="C34" t="s">
+        <v>314</v>
+      </c>
+      <c r="D34" t="s">
+        <v>315</v>
+      </c>
+      <c r="E34" s="3">
+        <v>39614</v>
+      </c>
+      <c r="F34" t="s">
+        <v>189</v>
+      </c>
+      <c r="G34" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" t="s">
+        <v>316</v>
+      </c>
+      <c r="D35" t="s">
+        <v>317</v>
+      </c>
+      <c r="E35" s="3">
+        <v>40071</v>
+      </c>
+      <c r="F35" t="s">
+        <v>220</v>
+      </c>
+      <c r="G35" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" t="s">
+        <v>318</v>
+      </c>
+      <c r="D36" t="s">
+        <v>319</v>
+      </c>
+      <c r="E36" s="3">
+        <v>26569</v>
+      </c>
+      <c r="F36" t="s">
+        <v>220</v>
+      </c>
+      <c r="G36" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>110</v>
+      </c>
+      <c r="C37" t="s">
+        <v>320</v>
+      </c>
+      <c r="D37" t="s">
+        <v>321</v>
+      </c>
+      <c r="E37" s="3">
+        <v>46731</v>
+      </c>
+      <c r="F37" t="s">
+        <v>220</v>
+      </c>
+      <c r="G37" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="7">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>136</v>
+      </c>
+      <c r="C38" t="s">
+        <v>322</v>
+      </c>
+      <c r="D38" t="s">
+        <v>323</v>
+      </c>
+      <c r="E38" s="3">
+        <v>21146</v>
+      </c>
+      <c r="F38" t="s">
+        <v>189</v>
+      </c>
+      <c r="G38" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" t="s">
+        <v>324</v>
+      </c>
+      <c r="D39" t="s">
+        <v>325</v>
+      </c>
+      <c r="E39" s="3">
+        <v>18140</v>
+      </c>
+      <c r="F39" t="s">
+        <v>189</v>
+      </c>
+      <c r="G39" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>158</v>
+      </c>
+      <c r="C40" t="s">
+        <v>326</v>
+      </c>
+      <c r="D40" t="s">
+        <v>327</v>
+      </c>
+      <c r="E40" s="3">
+        <v>33567</v>
+      </c>
+      <c r="F40" t="s">
+        <v>189</v>
+      </c>
+      <c r="G40" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" t="s">
+        <v>328</v>
+      </c>
+      <c r="D41" t="s">
+        <v>329</v>
+      </c>
+      <c r="E41" s="3">
+        <v>18722</v>
+      </c>
+      <c r="F41" t="s">
+        <v>220</v>
+      </c>
+      <c r="G41" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>147</v>
+      </c>
+      <c r="C42" t="s">
+        <v>330</v>
+      </c>
+      <c r="D42" t="s">
+        <v>331</v>
+      </c>
+      <c r="E42" s="3">
+        <v>23849</v>
+      </c>
+      <c r="F42" t="s">
+        <v>189</v>
+      </c>
+      <c r="G42" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" t="s">
+        <v>332</v>
+      </c>
+      <c r="D43" t="s">
+        <v>333</v>
+      </c>
+      <c r="E43" s="3">
+        <v>20794</v>
+      </c>
+      <c r="F43" t="s">
+        <v>189</v>
+      </c>
+      <c r="G43" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="7">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" t="s">
+        <v>334</v>
+      </c>
+      <c r="D44" t="s">
+        <v>335</v>
+      </c>
+      <c r="E44" s="3">
+        <v>31726</v>
+      </c>
+      <c r="F44" t="s">
+        <v>189</v>
+      </c>
+      <c r="G44" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="7">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" t="s">
+        <v>336</v>
+      </c>
+      <c r="D45" t="s">
+        <v>337</v>
+      </c>
+      <c r="E45" s="3">
+        <v>39384</v>
+      </c>
+      <c r="F45" t="s">
+        <v>189</v>
+      </c>
+      <c r="G45" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="7">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" t="s">
+        <v>338</v>
+      </c>
+      <c r="D46" t="s">
+        <v>339</v>
+      </c>
+      <c r="E46" s="3">
+        <v>32627</v>
+      </c>
+      <c r="F46" t="s">
+        <v>220</v>
+      </c>
+      <c r="G46" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="7">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>93</v>
+      </c>
+      <c r="C47" t="s">
+        <v>340</v>
+      </c>
+      <c r="D47" t="s">
+        <v>341</v>
+      </c>
+      <c r="E47" s="3">
+        <v>22924</v>
+      </c>
+      <c r="F47" t="s">
+        <v>189</v>
+      </c>
+      <c r="G47" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="7">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>125</v>
+      </c>
+      <c r="C48" t="s">
+        <v>342</v>
+      </c>
+      <c r="D48" t="s">
+        <v>343</v>
+      </c>
+      <c r="E48" s="3">
+        <v>24876</v>
+      </c>
+      <c r="F48" t="s">
+        <v>220</v>
+      </c>
+      <c r="G48" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="7">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>127</v>
+      </c>
+      <c r="C49" t="s">
+        <v>344</v>
+      </c>
+      <c r="D49" t="s">
+        <v>345</v>
+      </c>
+      <c r="E49" s="3">
+        <v>22410</v>
+      </c>
+      <c r="F49" t="s">
+        <v>220</v>
+      </c>
+      <c r="G49" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="7">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>89</v>
+      </c>
+      <c r="C50" t="s">
+        <v>346</v>
+      </c>
+      <c r="D50" t="s">
+        <v>347</v>
+      </c>
+      <c r="E50" s="3">
+        <v>38319</v>
+      </c>
+      <c r="F50" t="s">
+        <v>220</v>
+      </c>
+      <c r="G50" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="7">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>92</v>
+      </c>
+      <c r="C51" t="s">
+        <v>348</v>
+      </c>
+      <c r="D51" t="s">
+        <v>349</v>
+      </c>
+      <c r="E51" s="3">
+        <v>30055</v>
+      </c>
+      <c r="F51" t="s">
+        <v>189</v>
+      </c>
+      <c r="G51" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="7">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>37</v>
+      </c>
+      <c r="C52" t="s">
+        <v>350</v>
+      </c>
+      <c r="D52" t="s">
+        <v>351</v>
+      </c>
+      <c r="E52" s="3">
+        <v>38495</v>
+      </c>
+      <c r="F52" t="s">
+        <v>189</v>
+      </c>
+      <c r="G52" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="7">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>162</v>
+      </c>
+      <c r="C53" t="s">
+        <v>352</v>
+      </c>
+      <c r="D53" t="s">
+        <v>353</v>
+      </c>
+      <c r="E53" s="3">
+        <v>27912</v>
+      </c>
+      <c r="F53" t="s">
+        <v>189</v>
+      </c>
+      <c r="G53" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="7">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>71</v>
+      </c>
+      <c r="C54" t="s">
+        <v>354</v>
+      </c>
+      <c r="D54" t="s">
+        <v>355</v>
+      </c>
+      <c r="E54" s="3">
+        <v>28037</v>
+      </c>
+      <c r="F54" t="s">
+        <v>189</v>
+      </c>
+      <c r="G54" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="7">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>151</v>
+      </c>
+      <c r="C55" t="s">
+        <v>356</v>
+      </c>
+      <c r="D55" t="s">
+        <v>357</v>
+      </c>
+      <c r="E55" s="3">
+        <v>24015</v>
+      </c>
+      <c r="F55" t="s">
+        <v>220</v>
+      </c>
+      <c r="G55" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="7">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>95</v>
+      </c>
+      <c r="C56" t="s">
+        <v>358</v>
+      </c>
+      <c r="D56" t="s">
+        <v>359</v>
+      </c>
+      <c r="E56" s="3">
+        <v>22510</v>
+      </c>
+      <c r="F56" t="s">
+        <v>189</v>
+      </c>
+      <c r="G56" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="7">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>160</v>
+      </c>
+      <c r="C57" t="s">
+        <v>360</v>
+      </c>
+      <c r="D57" t="s">
+        <v>361</v>
+      </c>
+      <c r="E57" s="3">
+        <v>30164</v>
+      </c>
+      <c r="F57" t="s">
+        <v>189</v>
+      </c>
+      <c r="G57" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="7">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>81</v>
+      </c>
+      <c r="C58" t="s">
+        <v>362</v>
+      </c>
+      <c r="D58" t="s">
+        <v>363</v>
+      </c>
+      <c r="E58" s="3">
+        <v>31525</v>
+      </c>
+      <c r="F58" t="s">
+        <v>189</v>
+      </c>
+      <c r="G58" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="7">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>40</v>
+      </c>
+      <c r="C59" t="s">
+        <v>364</v>
+      </c>
+      <c r="D59" t="s">
+        <v>365</v>
+      </c>
+      <c r="E59" s="3">
+        <v>31398</v>
+      </c>
+      <c r="F59" t="s">
+        <v>220</v>
+      </c>
+      <c r="G59" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="7">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>30</v>
+      </c>
+      <c r="C60" t="s">
+        <v>366</v>
+      </c>
+      <c r="D60" t="s">
+        <v>367</v>
+      </c>
+      <c r="E60" s="3">
+        <v>29962</v>
+      </c>
+      <c r="F60" t="s">
+        <v>220</v>
+      </c>
+      <c r="G60" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="7">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" t="s">
+        <v>368</v>
+      </c>
+      <c r="D61" t="s">
+        <v>369</v>
+      </c>
+      <c r="E61" s="3">
+        <v>20861</v>
+      </c>
+      <c r="F61" t="s">
+        <v>220</v>
+      </c>
+      <c r="G61" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="7">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>121</v>
+      </c>
+      <c r="C62" t="s">
+        <v>370</v>
+      </c>
+      <c r="D62" t="s">
+        <v>371</v>
+      </c>
+      <c r="E62" s="3">
+        <v>28305</v>
+      </c>
+      <c r="F62" t="s">
+        <v>189</v>
+      </c>
+      <c r="G62" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="7">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>33</v>
+      </c>
+      <c r="C63" t="s">
+        <v>372</v>
+      </c>
+      <c r="D63" t="s">
+        <v>373</v>
+      </c>
+      <c r="E63" s="3">
+        <v>17683</v>
+      </c>
+      <c r="F63" t="s">
+        <v>220</v>
+      </c>
+      <c r="G63" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="7">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>140</v>
+      </c>
+      <c r="C64" t="s">
+        <v>374</v>
+      </c>
+      <c r="D64" t="s">
+        <v>375</v>
+      </c>
+      <c r="E64" s="3">
+        <v>19156</v>
+      </c>
+      <c r="F64" t="s">
+        <v>220</v>
+      </c>
+      <c r="G64" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="7">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>109</v>
+      </c>
+      <c r="C65" t="s">
+        <v>243</v>
+      </c>
+      <c r="D65" t="s">
+        <v>376</v>
+      </c>
+      <c r="E65" s="3">
+        <v>38126</v>
+      </c>
+      <c r="F65" t="s">
+        <v>189</v>
+      </c>
+      <c r="G65" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="7">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>166</v>
+      </c>
+      <c r="C66" t="s">
+        <v>377</v>
+      </c>
+      <c r="D66" t="s">
+        <v>378</v>
+      </c>
+      <c r="E66" s="3">
+        <v>39717</v>
+      </c>
+      <c r="F66" t="s">
+        <v>189</v>
+      </c>
+      <c r="G66" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="7">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>24</v>
+      </c>
+      <c r="C67" t="s">
+        <v>379</v>
+      </c>
+      <c r="D67" t="s">
+        <v>380</v>
+      </c>
+      <c r="E67" s="3">
+        <v>33191</v>
+      </c>
+      <c r="F67" t="s">
+        <v>220</v>
+      </c>
+      <c r="G67" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="7">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>45</v>
+      </c>
+      <c r="C68" t="s">
+        <v>381</v>
+      </c>
+      <c r="D68" t="s">
+        <v>382</v>
+      </c>
+      <c r="E68" s="3">
+        <v>22739</v>
+      </c>
+      <c r="F68" t="s">
+        <v>189</v>
+      </c>
+      <c r="G68" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="7">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>59</v>
+      </c>
+      <c r="C69" t="s">
+        <v>383</v>
+      </c>
+      <c r="D69" t="s">
+        <v>384</v>
+      </c>
+      <c r="E69" s="3">
+        <v>29633</v>
+      </c>
+      <c r="F69" t="s">
+        <v>189</v>
+      </c>
+      <c r="G69" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="7">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" t="s">
+        <v>385</v>
+      </c>
+      <c r="D70" t="s">
+        <v>386</v>
+      </c>
+      <c r="E70" s="3">
+        <v>24451</v>
+      </c>
+      <c r="F70" t="s">
+        <v>189</v>
+      </c>
+      <c r="G70" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="7">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>79</v>
+      </c>
+      <c r="C71" t="s">
+        <v>387</v>
+      </c>
+      <c r="D71" t="s">
+        <v>388</v>
+      </c>
+      <c r="E71" s="3">
+        <v>25773</v>
+      </c>
+      <c r="F71" t="s">
+        <v>189</v>
+      </c>
+      <c r="G71" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="7">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>97</v>
+      </c>
+      <c r="C72" t="s">
+        <v>389</v>
+      </c>
+      <c r="D72" t="s">
+        <v>390</v>
+      </c>
+      <c r="E72" s="3">
+        <v>29414</v>
+      </c>
+      <c r="F72" t="s">
+        <v>220</v>
+      </c>
+      <c r="G72" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="7">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>105</v>
+      </c>
+      <c r="C73" t="s">
+        <v>391</v>
+      </c>
+      <c r="D73" t="s">
+        <v>392</v>
+      </c>
+      <c r="E73" s="3">
+        <v>27902</v>
+      </c>
+      <c r="F73" t="s">
+        <v>220</v>
+      </c>
+      <c r="G73" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="7">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>91</v>
+      </c>
+      <c r="C74" t="s">
+        <v>393</v>
+      </c>
+      <c r="D74" t="s">
+        <v>394</v>
+      </c>
+      <c r="E74" s="4">
+        <v>40538</v>
+      </c>
+      <c r="F74" t="s">
+        <v>189</v>
+      </c>
+      <c r="G74" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="7">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>18</v>
+      </c>
+      <c r="C75" t="s">
+        <v>395</v>
+      </c>
+      <c r="D75" t="s">
+        <v>396</v>
+      </c>
+      <c r="E75" s="3">
+        <v>26952</v>
+      </c>
+      <c r="F75" t="s">
+        <v>220</v>
+      </c>
+      <c r="G75" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="7">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>129</v>
+      </c>
+      <c r="C76" t="s">
+        <v>397</v>
+      </c>
+      <c r="D76" t="s">
+        <v>398</v>
+      </c>
+      <c r="E76" s="3">
+        <v>26789</v>
+      </c>
+      <c r="F76" t="s">
+        <v>189</v>
+      </c>
+      <c r="G76" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="7">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>134</v>
+      </c>
+      <c r="C77" t="s">
+        <v>399</v>
+      </c>
+      <c r="D77" t="s">
+        <v>400</v>
+      </c>
+      <c r="E77" s="3">
+        <v>31984</v>
+      </c>
+      <c r="F77" t="s">
+        <v>189</v>
+      </c>
+      <c r="G77" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="7">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>5</v>
+      </c>
+      <c r="C78" t="s">
+        <v>401</v>
+      </c>
+      <c r="D78" t="s">
+        <v>402</v>
+      </c>
+      <c r="E78" s="3">
+        <v>31658</v>
+      </c>
+      <c r="F78" t="s">
+        <v>189</v>
+      </c>
+      <c r="G78" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="7">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>119</v>
+      </c>
+      <c r="C79" t="s">
+        <v>403</v>
+      </c>
+      <c r="D79" t="s">
+        <v>404</v>
+      </c>
+      <c r="E79" s="3">
+        <v>18470</v>
+      </c>
+      <c r="F79" t="s">
+        <v>220</v>
+      </c>
+      <c r="G79" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="7">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>133</v>
+      </c>
+      <c r="C80" t="s">
+        <v>405</v>
+      </c>
+      <c r="D80" t="s">
+        <v>406</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="F80" t="s">
+        <v>189</v>
+      </c>
+      <c r="G80" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="7">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>158</v>
+      </c>
+      <c r="C81" t="s">
+        <v>407</v>
+      </c>
+      <c r="D81" t="s">
+        <v>408</v>
+      </c>
+      <c r="E81" s="3">
+        <v>22604</v>
+      </c>
+      <c r="F81" t="s">
+        <v>189</v>
+      </c>
+      <c r="G81" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="7">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>77</v>
+      </c>
+      <c r="C82" t="s">
+        <v>409</v>
+      </c>
+      <c r="D82" t="s">
+        <v>410</v>
+      </c>
+      <c r="E82" s="3">
+        <v>27037</v>
+      </c>
+      <c r="F82" t="s">
+        <v>220</v>
+      </c>
+      <c r="G82" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="7">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>56</v>
+      </c>
+      <c r="C83" t="s">
+        <v>411</v>
+      </c>
+      <c r="D83" t="s">
+        <v>412</v>
+      </c>
+      <c r="E83" s="3">
+        <v>25703</v>
+      </c>
+      <c r="F83" t="s">
+        <v>220</v>
+      </c>
+      <c r="G83" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="7">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>107</v>
+      </c>
+      <c r="C84" t="s">
+        <v>413</v>
+      </c>
+      <c r="D84" t="s">
+        <v>414</v>
+      </c>
+      <c r="E84" s="3">
+        <v>25561</v>
+      </c>
+      <c r="F84" t="s">
+        <v>189</v>
+      </c>
+      <c r="G84" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="7">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>154</v>
+      </c>
+      <c r="C85" t="s">
+        <v>415</v>
+      </c>
+      <c r="D85" t="s">
+        <v>416</v>
+      </c>
+      <c r="E85" s="3">
+        <v>29091</v>
+      </c>
+      <c r="F85" t="s">
+        <v>220</v>
+      </c>
+      <c r="G85" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="7">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>85</v>
+      </c>
+      <c r="C86" t="s">
+        <v>417</v>
+      </c>
+      <c r="D86" t="s">
+        <v>418</v>
+      </c>
+      <c r="E86" s="3">
+        <v>28516</v>
+      </c>
+      <c r="F86" t="s">
+        <v>189</v>
+      </c>
+      <c r="G86" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="7">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>123</v>
+      </c>
+      <c r="C87" t="s">
+        <v>419</v>
+      </c>
+      <c r="D87" t="s">
+        <v>420</v>
+      </c>
+      <c r="E87" s="3">
+        <v>31784</v>
+      </c>
+      <c r="F87" t="s">
+        <v>220</v>
+      </c>
+      <c r="G87" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="7">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>153</v>
+      </c>
+      <c r="C88" t="s">
+        <v>421</v>
+      </c>
+      <c r="D88" t="s">
+        <v>422</v>
+      </c>
+      <c r="E88" s="4">
+        <v>40754</v>
+      </c>
+      <c r="F88" t="s">
+        <v>220</v>
+      </c>
+      <c r="G88" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="7">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>23</v>
+      </c>
+      <c r="C89" t="s">
+        <v>423</v>
+      </c>
+      <c r="D89" t="s">
+        <v>424</v>
+      </c>
+      <c r="E89" s="3">
+        <v>38861</v>
+      </c>
+      <c r="F89" t="s">
+        <v>220</v>
+      </c>
+      <c r="G89" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="7">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>9</v>
+      </c>
+      <c r="C90" t="s">
+        <v>425</v>
+      </c>
+      <c r="D90" t="s">
+        <v>426</v>
+      </c>
+      <c r="E90" s="3">
+        <v>32642</v>
+      </c>
+      <c r="F90" t="s">
+        <v>220</v>
+      </c>
+      <c r="G90" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="7">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>38</v>
+      </c>
+      <c r="C91" t="s">
+        <v>427</v>
+      </c>
+      <c r="D91" t="s">
+        <v>428</v>
+      </c>
+      <c r="E91" s="3">
+        <v>25481</v>
+      </c>
+      <c r="F91" t="s">
+        <v>220</v>
+      </c>
+      <c r="G91" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" s="7">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>104</v>
+      </c>
+      <c r="C92" t="s">
+        <v>429</v>
+      </c>
+      <c r="D92" t="s">
+        <v>430</v>
+      </c>
+      <c r="E92" s="3">
+        <v>38277</v>
+      </c>
+      <c r="F92" t="s">
+        <v>222</v>
+      </c>
+      <c r="G92" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="7">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>53</v>
+      </c>
+      <c r="C93" t="s">
+        <v>431</v>
+      </c>
+      <c r="D93" t="s">
+        <v>432</v>
+      </c>
+      <c r="E93" s="3">
+        <v>17738</v>
+      </c>
+      <c r="F93" t="s">
+        <v>189</v>
+      </c>
+      <c r="G93" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="7">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>20</v>
+      </c>
+      <c r="C94" t="s">
+        <v>433</v>
+      </c>
+      <c r="D94" t="s">
+        <v>434</v>
+      </c>
+      <c r="E94" s="3">
+        <v>38551</v>
+      </c>
+      <c r="F94" t="s">
+        <v>220</v>
+      </c>
+      <c r="G94" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="7">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>142</v>
+      </c>
+      <c r="C95" t="s">
+        <v>435</v>
+      </c>
+      <c r="D95" t="s">
+        <v>436</v>
+      </c>
+      <c r="E95" s="3">
+        <v>23209</v>
+      </c>
+      <c r="F95" t="s">
+        <v>220</v>
+      </c>
+      <c r="G95" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="7">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>151</v>
+      </c>
+      <c r="C96" t="s">
+        <v>437</v>
+      </c>
+      <c r="D96" t="s">
+        <v>438</v>
+      </c>
+      <c r="E96" s="3">
+        <v>38948</v>
+      </c>
+      <c r="F96" t="s">
+        <v>220</v>
+      </c>
+      <c r="G96" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="7">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>99</v>
+      </c>
+      <c r="C97" t="s">
+        <v>439</v>
+      </c>
+      <c r="D97" t="s">
+        <v>440</v>
+      </c>
+      <c r="E97" s="3">
+        <v>25382</v>
+      </c>
+      <c r="F97" t="s">
+        <v>220</v>
+      </c>
+      <c r="G97" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="7">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>164</v>
+      </c>
+      <c r="C98" t="s">
+        <v>441</v>
+      </c>
+      <c r="D98" t="s">
+        <v>442</v>
+      </c>
+      <c r="E98" s="3">
+        <v>27675</v>
+      </c>
+      <c r="F98" t="s">
+        <v>189</v>
+      </c>
+      <c r="G98" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="7">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>114</v>
+      </c>
+      <c r="C99" t="s">
+        <v>443</v>
+      </c>
+      <c r="D99" t="s">
+        <v>444</v>
+      </c>
+      <c r="E99" s="3">
+        <v>29803</v>
+      </c>
+      <c r="F99" t="s">
+        <v>189</v>
+      </c>
+      <c r="G99" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="7">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>90</v>
+      </c>
+      <c r="C100" t="s">
+        <v>445</v>
+      </c>
+      <c r="D100" t="s">
+        <v>446</v>
+      </c>
+      <c r="E100" s="3">
+        <v>19223</v>
+      </c>
+      <c r="F100" t="s">
+        <v>220</v>
+      </c>
+      <c r="G100" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="7">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>74</v>
+      </c>
+      <c r="C101" t="s">
+        <v>447</v>
+      </c>
+      <c r="D101" t="s">
+        <v>448</v>
+      </c>
+      <c r="E101" s="3">
+        <v>33711</v>
+      </c>
+      <c r="F101" t="s">
+        <v>220</v>
+      </c>
+      <c r="G101" t="s">
+        <v>216</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D8B9F0E-8FFC-4743-8C03-98D78646C655}">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>483</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D1" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C3" t="s">
+        <v>232</v>
+      </c>
+      <c r="D3" t="s">
+        <v>233</v>
+      </c>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D4" t="s">
+        <v>235</v>
+      </c>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D5" t="s">
+        <v>237</v>
+      </c>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C6" t="s">
+        <v>238</v>
+      </c>
+      <c r="D6" t="s">
+        <v>239</v>
+      </c>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C7" t="s">
+        <v>240</v>
+      </c>
+      <c r="D7" t="s">
+        <v>241</v>
+      </c>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C8" t="s">
+        <v>242</v>
+      </c>
+      <c r="D8" t="s">
+        <v>243</v>
+      </c>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>219</v>
+      </c>
+      <c r="C9" t="s">
+        <v>244</v>
+      </c>
+      <c r="D9" t="s">
+        <v>245</v>
+      </c>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>191</v>
+      </c>
+      <c r="C10" t="s">
+        <v>246</v>
+      </c>
+      <c r="D10" t="s">
+        <v>247</v>
+      </c>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>192</v>
+      </c>
+      <c r="C11" t="s">
+        <v>240</v>
+      </c>
+      <c r="D11" t="s">
+        <v>248</v>
+      </c>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>191</v>
+      </c>
+      <c r="C12" t="s">
+        <v>244</v>
+      </c>
+      <c r="D12" t="s">
+        <v>245</v>
+      </c>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>218</v>
+      </c>
+      <c r="C13" t="s">
+        <v>242</v>
+      </c>
+      <c r="D13" t="s">
+        <v>243</v>
+      </c>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>219</v>
+      </c>
+      <c r="C14" t="s">
+        <v>230</v>
+      </c>
+      <c r="D14" t="s">
+        <v>231</v>
+      </c>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E15" t="str">
+        <f t="shared" ref="E15:E19" si="0">_xlfn.CONCAT(B15, C15,D15)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E16" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E2:F14">
+    <sortCondition ref="E2:E14"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B07916B-927F-40C4-BE07-4FD93D7D5406}">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>482</v>
+      </c>
+      <c r="B1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2" t="s">
+        <v>452</v>
+      </c>
+      <c r="D2" t="s">
+        <v>453</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D3" t="s">
+        <v>455</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C4" t="s">
+        <v>456</v>
+      </c>
+      <c r="D4" t="s">
+        <v>457</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>226</v>
+      </c>
+      <c r="C5" t="s">
+        <v>458</v>
+      </c>
+      <c r="D5" t="s">
+        <v>459</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>226</v>
+      </c>
+      <c r="C6" t="s">
+        <v>460</v>
+      </c>
+      <c r="D6" t="s">
+        <v>461</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C7" t="s">
+        <v>462</v>
+      </c>
+      <c r="D7" t="s">
+        <v>463</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>226</v>
+      </c>
+      <c r="C8" t="s">
+        <v>464</v>
+      </c>
+      <c r="D8" t="s">
+        <v>465</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>194</v>
+      </c>
+      <c r="C9" t="s">
+        <v>466</v>
+      </c>
+      <c r="D9" t="s">
+        <v>467</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>193</v>
+      </c>
+      <c r="C10" t="s">
+        <v>240</v>
+      </c>
+      <c r="D10" t="s">
+        <v>468</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C11" t="s">
+        <v>246</v>
+      </c>
+      <c r="D11" t="s">
+        <v>469</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>193</v>
+      </c>
+      <c r="C12" t="s">
+        <v>470</v>
+      </c>
+      <c r="D12" t="s">
+        <v>471</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>227</v>
+      </c>
+      <c r="C13" t="s">
+        <v>472</v>
+      </c>
+      <c r="D13" t="s">
+        <v>473</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>225</v>
+      </c>
+      <c r="C14" t="s">
+        <v>474</v>
+      </c>
+      <c r="D14" t="s">
+        <v>479</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>194</v>
+      </c>
+      <c r="C15" t="s">
+        <v>475</v>
+      </c>
+      <c r="D15" t="s">
+        <v>476</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>227</v>
+      </c>
+      <c r="C16" t="s">
+        <v>477</v>
+      </c>
+      <c r="D16" t="s">
+        <v>478</v>
+      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="7"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E2:F16">
+    <sortCondition ref="E2:E16"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D7FEC57-2140-47AC-B21C-F4AFA671DC7D}">
+  <dimension ref="A1:G101"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>484</v>
+      </c>
+      <c r="B1" t="s">
+        <v>483</v>
+      </c>
+      <c r="C1" t="s">
+        <v>485</v>
+      </c>
+      <c r="D1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>42186</v>
+      </c>
+      <c r="F2" s="2">
+        <v>42188</v>
+      </c>
+      <c r="G2" s="2">
+        <v>42240</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" s="7">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>42187</v>
+      </c>
+      <c r="F3" s="2">
+        <v>42188</v>
+      </c>
+      <c r="G3" s="2">
+        <v>42277</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>42189</v>
+      </c>
+      <c r="F4" s="2">
+        <v>42191</v>
+      </c>
+      <c r="G4" s="2">
+        <v>42209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2">
+        <v>42196</v>
+      </c>
+      <c r="F5" s="2">
+        <v>42198</v>
+      </c>
+      <c r="G5" s="2">
+        <v>42273</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="7">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>42198</v>
+      </c>
+      <c r="F6" s="2">
+        <v>42201</v>
+      </c>
+      <c r="G6" s="2">
+        <v>42280</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" s="7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2">
+        <v>42205</v>
+      </c>
+      <c r="F7" s="2">
+        <v>42208</v>
+      </c>
+      <c r="G7" s="2">
+        <v>42412</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" s="7">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8" s="2">
+        <v>42219</v>
+      </c>
+      <c r="F8" s="2">
+        <v>42220</v>
+      </c>
+      <c r="G8" s="2">
+        <v>42220</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" s="7">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2">
+        <v>42231</v>
+      </c>
+      <c r="F9" s="2">
+        <v>42231</v>
+      </c>
+      <c r="G9" s="2">
+        <v>42239</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>11</v>
+      </c>
+      <c r="C10" s="7">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2">
+        <v>42233</v>
+      </c>
+      <c r="F10" s="2">
+        <v>42234</v>
+      </c>
+      <c r="G10" s="2">
+        <v>42296</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" s="7">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>7</v>
+      </c>
+      <c r="E11" s="2">
+        <v>42234</v>
+      </c>
+      <c r="F11" s="2">
+        <v>42236</v>
+      </c>
+      <c r="G11" s="2">
+        <v>42255</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12" s="7">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>8</v>
+      </c>
+      <c r="E12" s="2">
+        <v>42248</v>
+      </c>
+      <c r="F12" s="2">
+        <v>42248</v>
+      </c>
+      <c r="G12" s="2">
+        <v>42298</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" s="7">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13" s="2">
+        <v>42250</v>
+      </c>
+      <c r="F13" s="2">
+        <v>42251</v>
+      </c>
+      <c r="G13" s="2">
+        <v>42276</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" s="7">
+        <v>13</v>
+      </c>
+      <c r="D14">
+        <v>9</v>
+      </c>
+      <c r="E14" s="2">
+        <v>42251</v>
+      </c>
+      <c r="F14" s="2">
+        <v>42251</v>
+      </c>
+      <c r="G14" s="2">
+        <v>42289</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15" s="7">
+        <v>14</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
+      <c r="E15" s="2">
+        <v>42250</v>
+      </c>
+      <c r="F15" s="2">
+        <v>42252</v>
+      </c>
+      <c r="G15" s="2">
+        <v>42291</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="C16" s="7">
+        <v>15</v>
+      </c>
+      <c r="D16">
+        <v>11</v>
+      </c>
+      <c r="E16" s="2">
+        <v>42250</v>
+      </c>
+      <c r="F16" s="2">
+        <v>42252</v>
+      </c>
+      <c r="G16" s="2">
+        <v>42343</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17" s="7">
+        <v>16</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+      <c r="E17" s="2">
+        <v>42253</v>
+      </c>
+      <c r="F17" s="2">
+        <v>42255</v>
+      </c>
+      <c r="G17" s="2">
+        <v>42313</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18" s="7">
+        <v>17</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18" s="2">
+        <v>42254</v>
+      </c>
+      <c r="F18" s="2">
+        <v>42256</v>
+      </c>
+      <c r="G18" s="2">
+        <v>42322</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19" s="7">
+        <v>18</v>
+      </c>
+      <c r="D19">
+        <v>11</v>
+      </c>
+      <c r="E19" s="2">
+        <v>42271</v>
+      </c>
+      <c r="F19" s="2">
+        <v>42274</v>
+      </c>
+      <c r="G19" s="2">
+        <v>42341</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20" s="7">
+        <v>19</v>
+      </c>
+      <c r="D20">
+        <v>12</v>
+      </c>
+      <c r="E20" s="2">
+        <v>42279</v>
+      </c>
+      <c r="F20" s="2">
+        <v>42281</v>
+      </c>
+      <c r="G20" s="2">
+        <v>42286</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>10</v>
+      </c>
+      <c r="C21" s="7">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <v>13</v>
+      </c>
+      <c r="E21" s="2">
+        <v>42282</v>
+      </c>
+      <c r="F21" s="2">
+        <v>42283</v>
+      </c>
+      <c r="G21" s="2">
+        <v>42369</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>6</v>
+      </c>
+      <c r="C22" s="7">
+        <v>21</v>
+      </c>
+      <c r="D22">
+        <v>7</v>
+      </c>
+      <c r="E22" s="2">
+        <v>42291</v>
+      </c>
+      <c r="F22" s="2">
+        <v>42294</v>
+      </c>
+      <c r="G22" s="2">
+        <v>42358</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23" s="7">
+        <v>22</v>
+      </c>
+      <c r="D23">
+        <v>14</v>
+      </c>
+      <c r="E23" s="2">
+        <v>42293</v>
+      </c>
+      <c r="F23" s="2">
+        <v>42295</v>
+      </c>
+      <c r="G23" s="2">
+        <v>42303</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>9</v>
+      </c>
+      <c r="C24" s="7">
+        <v>23</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
+      </c>
+      <c r="E24" s="2">
+        <v>42300</v>
+      </c>
+      <c r="F24" s="2">
+        <v>42302</v>
+      </c>
+      <c r="G24" s="2">
+        <v>42343</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25" s="7">
+        <v>24</v>
+      </c>
+      <c r="D25">
+        <v>8</v>
+      </c>
+      <c r="E25" s="2">
+        <v>42301</v>
+      </c>
+      <c r="F25" s="2">
+        <v>42302</v>
+      </c>
+      <c r="G25" s="2">
+        <v>42659</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26" s="7">
+        <v>25</v>
+      </c>
+      <c r="D26">
+        <v>11</v>
+      </c>
+      <c r="E26" s="2">
+        <v>42316</v>
+      </c>
+      <c r="F26" s="2">
+        <v>42316</v>
+      </c>
+      <c r="G26" s="2">
+        <v>42372</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27" s="7">
+        <v>26</v>
+      </c>
+      <c r="D27">
+        <v>10</v>
+      </c>
+      <c r="E27" s="2">
+        <v>42317</v>
+      </c>
+      <c r="F27" s="2">
+        <v>42319</v>
+      </c>
+      <c r="G27" s="2">
+        <v>42408</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>11</v>
+      </c>
+      <c r="C28" s="7">
+        <v>27</v>
+      </c>
+      <c r="D28">
+        <v>8</v>
+      </c>
+      <c r="E28" s="2">
+        <v>42318</v>
+      </c>
+      <c r="F28" s="2">
+        <v>42320</v>
+      </c>
+      <c r="G28" s="2">
+        <v>42375</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" s="7">
+        <v>28</v>
+      </c>
+      <c r="D29">
+        <v>12</v>
+      </c>
+      <c r="E29" s="2">
+        <v>42323</v>
+      </c>
+      <c r="F29" s="2">
+        <v>42323</v>
+      </c>
+      <c r="G29" s="2">
+        <v>42350</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30" s="7">
+        <v>29</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" s="2">
+        <v>42325</v>
+      </c>
+      <c r="F30" s="2">
+        <v>42326</v>
+      </c>
+      <c r="G30" s="2">
+        <v>42389</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>12</v>
+      </c>
+      <c r="C31" s="7">
+        <v>30</v>
+      </c>
+      <c r="D31">
+        <v>11</v>
+      </c>
+      <c r="E31" s="2">
+        <v>42325</v>
+      </c>
+      <c r="F31" s="2">
+        <v>42328</v>
+      </c>
+      <c r="G31" s="2">
+        <v>42369</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32" s="7">
+        <v>31</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32" s="2">
+        <v>42333</v>
+      </c>
+      <c r="F32" s="2">
+        <v>42336</v>
+      </c>
+      <c r="G32" s="2">
+        <v>42421</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33" s="7">
+        <v>32</v>
+      </c>
+      <c r="D33">
+        <v>9</v>
+      </c>
+      <c r="E33" s="2">
+        <v>42340</v>
+      </c>
+      <c r="F33" s="2">
+        <v>42341</v>
+      </c>
+      <c r="G33" s="2">
+        <v>42387</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>9</v>
+      </c>
+      <c r="C34" s="7">
+        <v>33</v>
+      </c>
+      <c r="D34">
+        <v>10</v>
+      </c>
+      <c r="E34" s="2">
+        <v>42343</v>
+      </c>
+      <c r="F34" s="2">
+        <v>42344</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>11</v>
+      </c>
+      <c r="C35" s="7">
+        <v>34</v>
+      </c>
+      <c r="D35">
+        <v>10</v>
+      </c>
+      <c r="E35" s="2">
+        <v>42343</v>
+      </c>
+      <c r="F35" s="2">
+        <v>42345</v>
+      </c>
+      <c r="G35" s="2">
+        <v>42425</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="C36" s="7">
+        <v>35</v>
+      </c>
+      <c r="D36">
+        <v>5</v>
+      </c>
+      <c r="E36" s="2">
+        <v>42346</v>
+      </c>
+      <c r="F36" s="2">
+        <v>42346</v>
+      </c>
+      <c r="G36" s="2">
+        <v>42418</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>5</v>
+      </c>
+      <c r="C37" s="7">
+        <v>36</v>
+      </c>
+      <c r="D37">
+        <v>8</v>
+      </c>
+      <c r="E37" s="2">
+        <v>42368</v>
+      </c>
+      <c r="F37" s="2">
+        <v>42369</v>
+      </c>
+      <c r="G37" s="2">
+        <v>42380</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38" s="7">
+        <v>37</v>
+      </c>
+      <c r="D38">
+        <v>5</v>
+      </c>
+      <c r="E38" s="2">
+        <v>42371</v>
+      </c>
+      <c r="F38" s="2">
+        <v>42371</v>
+      </c>
+      <c r="G38" s="2">
+        <v>42409</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>5</v>
+      </c>
+      <c r="C39" s="7">
+        <v>38</v>
+      </c>
+      <c r="D39">
+        <v>15</v>
+      </c>
+      <c r="E39" s="2">
+        <v>42372</v>
+      </c>
+      <c r="F39" s="2">
+        <v>42372</v>
+      </c>
+      <c r="G39" s="2">
+        <v>42402</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>10</v>
+      </c>
+      <c r="C40" s="7">
+        <v>39</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40" s="2">
+        <v>42369</v>
+      </c>
+      <c r="F40" s="2">
+        <v>42372</v>
+      </c>
+      <c r="G40" s="2">
+        <v>42411</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>6</v>
+      </c>
+      <c r="C41" s="7">
+        <v>40</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41" s="2">
+        <v>42373</v>
+      </c>
+      <c r="F41" s="2">
+        <v>42375</v>
+      </c>
+      <c r="G41" s="2">
+        <v>42427</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>11</v>
+      </c>
+      <c r="C42" s="7">
+        <v>41</v>
+      </c>
+      <c r="D42">
+        <v>9</v>
+      </c>
+      <c r="E42" s="2">
+        <v>42375</v>
+      </c>
+      <c r="F42" s="2">
+        <v>42377</v>
+      </c>
+      <c r="G42" s="2">
+        <v>42429</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>5</v>
+      </c>
+      <c r="C43" s="7">
+        <v>42</v>
+      </c>
+      <c r="D43">
+        <v>13</v>
+      </c>
+      <c r="E43" s="2">
+        <v>42381</v>
+      </c>
+      <c r="F43" s="2">
+        <v>42383</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" s="7">
+        <v>43</v>
+      </c>
+      <c r="D44">
+        <v>11</v>
+      </c>
+      <c r="E44" s="2">
+        <v>42391</v>
+      </c>
+      <c r="F44" s="2">
+        <v>42392</v>
+      </c>
+      <c r="G44" s="2">
+        <v>42452</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45" s="7">
+        <v>44</v>
+      </c>
+      <c r="D45">
+        <v>8</v>
+      </c>
+      <c r="E45" s="2">
+        <v>42393</v>
+      </c>
+      <c r="F45" s="2">
+        <v>42396</v>
+      </c>
+      <c r="G45" s="2">
+        <v>42434</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>6</v>
+      </c>
+      <c r="C46" s="7">
+        <v>45</v>
+      </c>
+      <c r="D46">
+        <v>7</v>
+      </c>
+      <c r="E46" s="2">
+        <v>42402</v>
+      </c>
+      <c r="F46" s="2">
+        <v>42403</v>
+      </c>
+      <c r="G46" s="2">
+        <v>42438</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>13</v>
+      </c>
+      <c r="C47" s="7">
+        <v>46</v>
+      </c>
+      <c r="D47">
+        <v>13</v>
+      </c>
+      <c r="E47" s="2">
+        <v>42401</v>
+      </c>
+      <c r="F47" s="2">
+        <v>42404</v>
+      </c>
+      <c r="G47" s="2">
+        <v>42451</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>9</v>
+      </c>
+      <c r="C48" s="7">
+        <v>47</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48" s="2">
+        <v>42405</v>
+      </c>
+      <c r="F48" s="2">
+        <v>42407</v>
+      </c>
+      <c r="G48" s="2">
+        <v>42445</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>12</v>
+      </c>
+      <c r="C49" s="7">
+        <v>48</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="E49" s="2">
+        <v>42407</v>
+      </c>
+      <c r="F49" s="2">
+        <v>42408</v>
+      </c>
+      <c r="G49" s="2">
+        <v>42410</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>2</v>
+      </c>
+      <c r="C50" s="7">
+        <v>49</v>
+      </c>
+      <c r="D50">
+        <v>8</v>
+      </c>
+      <c r="E50" s="2">
+        <v>42414</v>
+      </c>
+      <c r="F50" s="2">
+        <v>42415</v>
+      </c>
+      <c r="G50" s="2">
+        <v>42619</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>5</v>
+      </c>
+      <c r="C51" s="7">
+        <v>50</v>
+      </c>
+      <c r="D51">
+        <v>3</v>
+      </c>
+      <c r="E51" s="2">
+        <v>42420</v>
+      </c>
+      <c r="F51" s="2">
+        <v>42421</v>
+      </c>
+      <c r="G51" s="2">
+        <v>42485</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>9</v>
+      </c>
+      <c r="C52" s="7">
+        <v>51</v>
+      </c>
+      <c r="D52">
+        <v>10</v>
+      </c>
+      <c r="E52" s="2">
+        <v>42424</v>
+      </c>
+      <c r="F52" s="2">
+        <v>42424</v>
+      </c>
+      <c r="G52" s="2">
+        <v>42445</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="C53" s="7">
+        <v>52</v>
+      </c>
+      <c r="D53">
+        <v>3</v>
+      </c>
+      <c r="E53" s="2">
+        <v>42421</v>
+      </c>
+      <c r="F53" s="2">
+        <v>42424</v>
+      </c>
+      <c r="G53" s="2">
+        <v>42506</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>6</v>
+      </c>
+      <c r="C54" s="7">
+        <v>53</v>
+      </c>
+      <c r="D54">
+        <v>9</v>
+      </c>
+      <c r="E54" s="2">
+        <v>42424</v>
+      </c>
+      <c r="F54" s="2">
+        <v>42425</v>
+      </c>
+      <c r="G54" s="2">
+        <v>42497</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>8</v>
+      </c>
+      <c r="C55" s="7">
+        <v>54</v>
+      </c>
+      <c r="D55">
+        <v>7</v>
+      </c>
+      <c r="E55" s="2">
+        <v>42426</v>
+      </c>
+      <c r="F55" s="2">
+        <v>42427</v>
+      </c>
+      <c r="G55" s="2">
+        <v>42616</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>13</v>
+      </c>
+      <c r="C56" s="7">
+        <v>55</v>
+      </c>
+      <c r="D56">
+        <v>9</v>
+      </c>
+      <c r="E56" s="2">
+        <v>42434</v>
+      </c>
+      <c r="F56" s="2">
+        <v>42437</v>
+      </c>
+      <c r="G56" s="2">
+        <v>42457</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57" s="7">
+        <v>56</v>
+      </c>
+      <c r="D57">
+        <v>5</v>
+      </c>
+      <c r="E57" s="2">
+        <v>42438</v>
+      </c>
+      <c r="F57" s="2">
+        <v>42438</v>
+      </c>
+      <c r="G57" s="2">
+        <v>42519</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>11</v>
+      </c>
+      <c r="C58" s="7">
+        <v>57</v>
+      </c>
+      <c r="D58">
+        <v>6</v>
+      </c>
+      <c r="E58" s="2">
+        <v>42437</v>
+      </c>
+      <c r="F58" s="2">
+        <v>42440</v>
+      </c>
+      <c r="G58" s="2">
+        <v>42498</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <v>5</v>
+      </c>
+      <c r="C59" s="7">
+        <v>58</v>
+      </c>
+      <c r="D59">
+        <v>12</v>
+      </c>
+      <c r="E59" s="2">
+        <v>42449</v>
+      </c>
+      <c r="F59" s="2">
+        <v>42450</v>
+      </c>
+      <c r="G59" s="2">
+        <v>42450</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B60">
+        <v>5</v>
+      </c>
+      <c r="C60" s="7">
+        <v>59</v>
+      </c>
+      <c r="D60">
+        <v>3</v>
+      </c>
+      <c r="E60" s="2">
+        <v>42449</v>
+      </c>
+      <c r="F60" s="2">
+        <v>42450</v>
+      </c>
+      <c r="G60" s="2">
+        <v>42506</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <v>11</v>
+      </c>
+      <c r="C61" s="7">
+        <v>60</v>
+      </c>
+      <c r="D61">
+        <v>2</v>
+      </c>
+      <c r="E61" s="2">
+        <v>42454</v>
+      </c>
+      <c r="F61" s="2">
+        <v>42457</v>
+      </c>
+      <c r="G61" s="2">
+        <v>42472</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <v>11</v>
+      </c>
+      <c r="C62" s="7">
+        <v>61</v>
+      </c>
+      <c r="D62">
+        <v>2</v>
+      </c>
+      <c r="E62" s="2">
+        <v>42457</v>
+      </c>
+      <c r="F62" s="2">
+        <v>42457</v>
+      </c>
+      <c r="G62" s="2">
+        <v>42476</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63" s="7">
+        <v>62</v>
+      </c>
+      <c r="D63">
+        <v>6</v>
+      </c>
+      <c r="E63" s="2">
+        <v>42455</v>
+      </c>
+      <c r="F63" s="2">
+        <v>42458</v>
+      </c>
+      <c r="G63" s="2">
+        <v>42502</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <v>9</v>
+      </c>
+      <c r="C64" s="7">
+        <v>63</v>
+      </c>
+      <c r="D64">
+        <v>9</v>
+      </c>
+      <c r="E64" s="2">
+        <v>42457</v>
+      </c>
+      <c r="F64" s="2">
+        <v>42459</v>
+      </c>
+      <c r="G64" s="2">
+        <v>42508</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <v>10</v>
+      </c>
+      <c r="C65" s="7">
+        <v>64</v>
+      </c>
+      <c r="D65">
+        <v>14</v>
+      </c>
+      <c r="E65" s="2">
+        <v>42458</v>
+      </c>
+      <c r="F65" s="2">
+        <v>42461</v>
+      </c>
+      <c r="G65" s="2">
+        <v>42505</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <v>6</v>
+      </c>
+      <c r="C66" s="7">
+        <v>65</v>
+      </c>
+      <c r="D66">
+        <v>14</v>
+      </c>
+      <c r="E66" s="2">
+        <v>42464</v>
+      </c>
+      <c r="F66" s="2">
+        <v>42465</v>
+      </c>
+      <c r="G66" s="2">
+        <v>42523</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>4</v>
+      </c>
+      <c r="C67" s="7">
+        <v>66</v>
+      </c>
+      <c r="D67">
+        <v>15</v>
+      </c>
+      <c r="E67" s="2">
+        <v>42469</v>
+      </c>
+      <c r="F67" s="2">
+        <v>42469</v>
+      </c>
+      <c r="G67" s="2">
+        <v>42531</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <v>11</v>
+      </c>
+      <c r="C68" s="7">
+        <v>67</v>
+      </c>
+      <c r="D68">
+        <v>13</v>
+      </c>
+      <c r="E68" s="2">
+        <v>42472</v>
+      </c>
+      <c r="F68" s="2">
+        <v>42475</v>
+      </c>
+      <c r="G68" s="2">
+        <v>42559</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69" s="7">
+        <v>68</v>
+      </c>
+      <c r="D69">
+        <v>4</v>
+      </c>
+      <c r="E69" s="2">
+        <v>42476</v>
+      </c>
+      <c r="F69" s="2">
+        <v>42478</v>
+      </c>
+      <c r="G69" s="2">
+        <v>42486</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B70">
+        <v>12</v>
+      </c>
+      <c r="C70" s="7">
+        <v>69</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70" s="2">
+        <v>42478</v>
+      </c>
+      <c r="F70" s="2">
+        <v>42479</v>
+      </c>
+      <c r="G70" s="2">
+        <v>42551</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B71">
+        <v>9</v>
+      </c>
+      <c r="C71" s="7">
+        <v>70</v>
+      </c>
+      <c r="D71">
+        <v>4</v>
+      </c>
+      <c r="E71" s="2">
+        <v>42478</v>
+      </c>
+      <c r="F71" s="2">
+        <v>42480</v>
+      </c>
+      <c r="G71" s="2">
+        <v>42499</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B72">
+        <v>9</v>
+      </c>
+      <c r="C72" s="7">
+        <v>71</v>
+      </c>
+      <c r="D72">
+        <v>13</v>
+      </c>
+      <c r="E72" s="2">
+        <v>42479</v>
+      </c>
+      <c r="F72" s="2">
+        <v>42480</v>
+      </c>
+      <c r="G72" s="2">
+        <v>42535</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B73">
+        <v>4</v>
+      </c>
+      <c r="C73" s="7">
+        <v>72</v>
+      </c>
+      <c r="D73">
+        <v>2</v>
+      </c>
+      <c r="E73" s="2">
+        <v>42478</v>
+      </c>
+      <c r="F73" s="2">
+        <v>42480</v>
+      </c>
+      <c r="G73" s="2">
+        <v>42552</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B74">
+        <v>4</v>
+      </c>
+      <c r="C74" s="7">
+        <v>73</v>
+      </c>
+      <c r="D74">
+        <v>14</v>
+      </c>
+      <c r="E74" s="2">
+        <v>42480</v>
+      </c>
+      <c r="F74" s="2">
+        <v>42482</v>
+      </c>
+      <c r="G74" s="2">
+        <v>42568</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B75">
+        <v>10</v>
+      </c>
+      <c r="C75" s="7">
+        <v>74</v>
+      </c>
+      <c r="D75">
+        <v>11</v>
+      </c>
+      <c r="E75" s="2">
+        <v>42482</v>
+      </c>
+      <c r="F75" s="2">
+        <v>42485</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B76">
+        <v>9</v>
+      </c>
+      <c r="C76" s="7">
+        <v>75</v>
+      </c>
+      <c r="D76">
+        <v>3</v>
+      </c>
+      <c r="E76" s="2">
+        <v>42486</v>
+      </c>
+      <c r="F76" s="2">
+        <v>42487</v>
+      </c>
+      <c r="G76" s="2">
+        <v>42535</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B77">
+        <v>11</v>
+      </c>
+      <c r="C77" s="7">
+        <v>76</v>
+      </c>
+      <c r="D77">
+        <v>2</v>
+      </c>
+      <c r="E77" s="2">
+        <v>42488</v>
+      </c>
+      <c r="F77" s="2">
+        <v>42489</v>
+      </c>
+      <c r="G77" s="2">
+        <v>42559</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B78">
+        <v>4</v>
+      </c>
+      <c r="C78" s="7">
+        <v>77</v>
+      </c>
+      <c r="D78">
+        <v>2</v>
+      </c>
+      <c r="E78" s="2">
+        <v>42494</v>
+      </c>
+      <c r="F78" s="2">
+        <v>42494</v>
+      </c>
+      <c r="G78" s="2">
+        <v>42525</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B79">
+        <v>1</v>
+      </c>
+      <c r="C79" s="7">
+        <v>78</v>
+      </c>
+      <c r="D79">
+        <v>12</v>
+      </c>
+      <c r="E79" s="2">
+        <v>42492</v>
+      </c>
+      <c r="F79" s="2">
+        <v>42495</v>
+      </c>
+      <c r="G79" s="2">
+        <v>42545</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B80">
+        <v>1</v>
+      </c>
+      <c r="C80" s="7">
+        <v>79</v>
+      </c>
+      <c r="D80">
+        <v>8</v>
+      </c>
+      <c r="E80" s="2">
+        <v>42504</v>
+      </c>
+      <c r="F80" s="2">
+        <v>42506</v>
+      </c>
+      <c r="G80" s="2">
+        <v>42539</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <v>12</v>
+      </c>
+      <c r="C81" s="7">
+        <v>80</v>
+      </c>
+      <c r="D81">
+        <v>15</v>
+      </c>
+      <c r="E81" s="2">
+        <v>42513</v>
+      </c>
+      <c r="F81" s="2">
+        <v>42514</v>
+      </c>
+      <c r="G81" s="2">
+        <v>42606</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B82">
+        <v>10</v>
+      </c>
+      <c r="C82" s="7">
+        <v>81</v>
+      </c>
+      <c r="D82">
+        <v>9</v>
+      </c>
+      <c r="E82" s="2">
+        <v>42516</v>
+      </c>
+      <c r="F82" s="2">
+        <v>42517</v>
+      </c>
+      <c r="G82" s="2">
+        <v>42563</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B83">
+        <v>4</v>
+      </c>
+      <c r="C83" s="7">
+        <v>82</v>
+      </c>
+      <c r="D83">
+        <v>6</v>
+      </c>
+      <c r="E83" s="2">
+        <v>42525</v>
+      </c>
+      <c r="F83" s="2">
+        <v>42528</v>
+      </c>
+      <c r="G83" s="2">
+        <v>42530</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B84">
+        <v>5</v>
+      </c>
+      <c r="C84" s="7">
+        <v>83</v>
+      </c>
+      <c r="D84">
+        <v>2</v>
+      </c>
+      <c r="E84" s="2">
+        <v>42536</v>
+      </c>
+      <c r="F84" s="2">
+        <v>42538</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B85">
+        <v>12</v>
+      </c>
+      <c r="C85" s="7">
+        <v>84</v>
+      </c>
+      <c r="D85">
+        <v>7</v>
+      </c>
+      <c r="E85" s="2">
+        <v>42537</v>
+      </c>
+      <c r="F85" s="2">
+        <v>42538</v>
+      </c>
+      <c r="G85" s="2">
+        <v>42608</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B86">
+        <v>9</v>
+      </c>
+      <c r="C86" s="7">
+        <v>85</v>
+      </c>
+      <c r="D86">
+        <v>9</v>
+      </c>
+      <c r="E86" s="2">
+        <v>42539</v>
+      </c>
+      <c r="F86" s="2">
+        <v>42541</v>
+      </c>
+      <c r="G86" s="2">
+        <v>42574</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B87">
+        <v>3</v>
+      </c>
+      <c r="C87" s="7">
+        <v>86</v>
+      </c>
+      <c r="D87">
+        <v>15</v>
+      </c>
+      <c r="E87" s="2">
+        <v>42540</v>
+      </c>
+      <c r="F87" s="2">
+        <v>42543</v>
+      </c>
+      <c r="G87" s="2">
+        <v>42615</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B88">
+        <v>5</v>
+      </c>
+      <c r="C88" s="7">
+        <v>87</v>
+      </c>
+      <c r="D88">
+        <v>10</v>
+      </c>
+      <c r="E88" s="2">
+        <v>42544</v>
+      </c>
+      <c r="F88" s="2">
+        <v>42544</v>
+      </c>
+      <c r="G88" s="2">
+        <v>42615</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B89">
+        <v>4</v>
+      </c>
+      <c r="C89" s="7">
+        <v>88</v>
+      </c>
+      <c r="D89">
+        <v>8</v>
+      </c>
+      <c r="E89" s="2">
+        <v>42543</v>
+      </c>
+      <c r="F89" s="2">
+        <v>42545</v>
+      </c>
+      <c r="G89" s="2">
+        <v>42568</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B90">
+        <v>9</v>
+      </c>
+      <c r="C90" s="7">
+        <v>89</v>
+      </c>
+      <c r="D90">
+        <v>13</v>
+      </c>
+      <c r="E90" s="2">
+        <v>42546</v>
+      </c>
+      <c r="F90" s="2">
+        <v>42548</v>
+      </c>
+      <c r="G90" s="2">
+        <v>42567</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B91">
+        <v>3</v>
+      </c>
+      <c r="C91" s="7">
+        <v>90</v>
+      </c>
+      <c r="D91">
+        <v>13</v>
+      </c>
+      <c r="E91" s="2">
+        <v>42558</v>
+      </c>
+      <c r="F91" s="2">
+        <v>42558</v>
+      </c>
+      <c r="G91" s="2">
+        <v>42635</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B92">
+        <v>10</v>
+      </c>
+      <c r="C92" s="7">
+        <v>91</v>
+      </c>
+      <c r="D92">
+        <v>14</v>
+      </c>
+      <c r="E92" s="2">
+        <v>42565</v>
+      </c>
+      <c r="F92" s="2">
+        <v>42568</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <v>9</v>
+      </c>
+      <c r="C93" s="7">
+        <v>92</v>
+      </c>
+      <c r="D93">
+        <v>11</v>
+      </c>
+      <c r="E93" s="2">
+        <v>42566</v>
+      </c>
+      <c r="F93" s="2">
+        <v>42568</v>
+      </c>
+      <c r="G93" s="2">
+        <v>42615</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>2</v>
+      </c>
+      <c r="C94" s="7">
+        <v>93</v>
+      </c>
+      <c r="D94">
+        <v>14</v>
+      </c>
+      <c r="E94" s="2">
+        <v>42570</v>
+      </c>
+      <c r="F94" s="2">
+        <v>42571</v>
+      </c>
+      <c r="G94" s="2">
+        <v>42660</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B95">
+        <v>11</v>
+      </c>
+      <c r="C95" s="7">
+        <v>94</v>
+      </c>
+      <c r="D95">
+        <v>13</v>
+      </c>
+      <c r="E95" s="2">
+        <v>42572</v>
+      </c>
+      <c r="F95" s="2">
+        <v>42574</v>
+      </c>
+      <c r="G95" s="2">
+        <v>42574</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B96">
+        <v>1</v>
+      </c>
+      <c r="C96" s="7">
+        <v>95</v>
+      </c>
+      <c r="D96">
+        <v>10</v>
+      </c>
+      <c r="E96" s="2">
+        <v>42572</v>
+      </c>
+      <c r="F96" s="2">
+        <v>42575</v>
+      </c>
+      <c r="G96" s="2">
+        <v>42659</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B97">
+        <v>4</v>
+      </c>
+      <c r="C97" s="7">
+        <v>96</v>
+      </c>
+      <c r="D97">
+        <v>1</v>
+      </c>
+      <c r="E97" s="2">
+        <v>42574</v>
+      </c>
+      <c r="F97" s="2">
+        <v>42577</v>
+      </c>
+      <c r="G97" s="2">
+        <v>42636</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B98">
+        <v>10</v>
+      </c>
+      <c r="C98" s="7">
+        <v>97</v>
+      </c>
+      <c r="D98">
+        <v>2</v>
+      </c>
+      <c r="E98" s="2">
+        <v>42578</v>
+      </c>
+      <c r="F98" s="2">
+        <v>42578</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B99">
+        <v>1</v>
+      </c>
+      <c r="C99" s="7">
+        <v>98</v>
+      </c>
+      <c r="D99">
+        <v>12</v>
+      </c>
+      <c r="E99" s="2">
+        <v>42592</v>
+      </c>
+      <c r="F99" s="2">
+        <v>42592</v>
+      </c>
+      <c r="G99" s="2">
+        <v>42606</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B100">
+        <v>11</v>
+      </c>
+      <c r="C100" s="7">
+        <v>99</v>
+      </c>
+      <c r="D100">
+        <v>11</v>
+      </c>
+      <c r="E100" s="2">
+        <v>42591</v>
+      </c>
+      <c r="F100" s="2">
+        <v>42594</v>
+      </c>
+      <c r="G100" s="2">
+        <v>42636</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B101">
+        <v>2</v>
+      </c>
+      <c r="C101" s="7">
+        <v>100</v>
+      </c>
+      <c r="D101">
+        <v>12</v>
+      </c>
+      <c r="E101" s="2">
+        <v>42593</v>
+      </c>
+      <c r="F101" s="2">
+        <v>42595</v>
+      </c>
+      <c r="G101" s="2">
+        <v>42645</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B2330"/>
   <sheetViews>

</xml_diff>